<commit_message>
Fix on info panel padding, new data in master.
</commit_message>
<xml_diff>
--- a/Master Info.xlsx
+++ b/Master Info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryansmith/Documents/Coding/topomapper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5C9D89-E7D7-9340-8752-C20E25FFE828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3D14E7-5FA9-3E42-A209-6E7E8C12C936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{1807FE50-C9A7-E24A-AB34-CDD2C78B0884}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{79D767BE-4211-C647-B28B-E0169FEB63DF}" name="streetInfo" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/bryansmith/Documents/Coding/topomapper/streetInfo.csv" delimiter="$">
+    <textPr sourceFile="/Users/bryansmith/Documents/Coding/topomapper/streetInfo.csv" delimiter="$">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="424">
   <si>
     <t xml:space="preserve">Alexandra Street </t>
   </si>
@@ -426,9 +426,6 @@
     <t xml:space="preserve">Flinders Street </t>
   </si>
   <si>
-    <t xml:space="preserve"> Named for Matthew Flinders, explorer of what is now called Australia, wrote "A Voyage to Terra Australis" which was published just before his death (Mathew, 2008, p. 49). Macintyre (2004) suggests that it was Flinders who came up with the name Australia since it was, in Flinders' words, "more agreeable to the ear" (p. 50). </t>
-  </si>
-  <si>
     <t xml:space="preserve">Francis Street </t>
   </si>
   <si>
@@ -1131,9 +1128,6 @@
     <t xml:space="preserve">Sturt Street </t>
   </si>
   <si>
-    <t xml:space="preserve"> Named for Captain Charles Sturt, one time Surveyor General of South Australia (Mathew, 2008, p. 115). </t>
-  </si>
-  <si>
     <t xml:space="preserve">Styx Street </t>
   </si>
   <si>
@@ -1306,13 +1300,37 @@
   </si>
   <si>
     <t>Mathew, J. (2008). &lt;i&gt;Highways and Byways: The Origin of Townsville Street Names&lt;/i&gt; (Revised ed.). Townsville, QLD: Townsville Library Service.</t>
+  </si>
+  <si>
+    <t>Br&amp;eacute;elle, D. (2013). Matthew Flinders's Australian toponymy and its British connections. &lt;i&gt;The Journal of the Hakluyt Society&lt;/i&gt;, 1–41.&lt;p&gt;&lt;/p&gt;Macintyre, S. (2004). &lt;i&gt;A Concise History of Australia&lt;/i&gt; (2nd ed.). Port Melbourne, VIC: Cambridge University Press.&lt;p&gt;&lt;/p&gt;Mathew, J. (2008). &lt;i&gt;Highways and Byways: The Origin of Townsville Street Names&lt;/i&gt; (Revised ed.). Townsville, QLD: Townsville Library Service.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Named for Matthew Flinders, explorer of what is now called Australia, wrote "A Voyage to Terra Australis" which was published just before his death (Mathew, 2008, p. 49). Macintyre (2004) suggests that it was Flinders who came up with the name Australia since it was, in Flinders' words, "more agreeable to the ear" (p. 50). Beyond the name of the continent itself, Flinders was a prolific namer, with more than 300 of his original names still in use (Br&amp;eacute;elle, 2013).</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Image secured</t>
+  </si>
+  <si>
+    <t>Something is going on here, needs to be addressed</t>
+  </si>
+  <si>
+    <t>Dowling, P. (2017). What Charles Sturt saw in 1830 – syphilis beyond the colonial boundaries? &lt;i&gt;Health and History, 19&lt;/i&gt;(1), 44–59.&lt;p&gt;&lt;/p&gt;Mathew, J. (2008). &lt;i&gt;Highways and Byways: The Origin of Townsville Street Names&lt;/i&gt; (Revised ed.). Townsville, QLD: Townsville Library Service.</t>
+  </si>
+  <si>
+    <t>Bolstered</t>
+  </si>
+  <si>
+    <t>Named for Captain Charles Sturt, one time Surveyor General of South Australia (Mathew, 2008, p. 115). A well traveled explorer, Sturt made many journeys inland, helping to map the interior. During one such journey, Dowling (2017) argues, Sturt noticed the spread of syphilis, one of the sexually transmitted STIs brought over by Europeans. To learn more, consider Sturt's writings about two expeditions inland: &lt;a href='https://books.google.com.au/books?hl=en&amp;lr=&amp;id=nMDCDwAAQBAJ&amp;oi=fnd&amp;pg=PT8&amp;dq=charles+sturt&amp;ots=l9oaADIRFt&amp;sig=Uc2JuFkj7Wb678CM-3tQJ-mATAw&amp;redir_esc=y#v=onepage&amp;q=charles%20sturt&amp;f=false'&gt;source&lt;/a&gt;.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1320,8 +1338,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1331,6 +1356,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1344,17 +1380,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1671,10 +1720,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC5444A-5FE5-E14D-8DB4-EE518C4047AC}">
-  <dimension ref="A1:D228"/>
+  <dimension ref="A1:F228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="760" topLeftCell="A181" activePane="bottomLeft"/>
+      <selection activeCell="E199" sqref="E199"/>
+      <selection pane="bottomLeft" activeCell="B199" sqref="B199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1682,23 +1733,27 @@
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="140.83203125" customWidth="1"/>
     <col min="3" max="3" width="100.1640625" customWidth="1"/>
+    <col min="5" max="5" width="43.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1706,13 +1761,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1720,13 +1775,13 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1734,13 +1789,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1748,27 +1803,27 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1776,13 +1831,13 @@
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1790,13 +1845,13 @@
         <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1804,13 +1859,13 @@
         <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1818,13 +1873,13 @@
         <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1832,13 +1887,13 @@
         <v>24</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1846,13 +1901,13 @@
         <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1860,13 +1915,13 @@
         <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1874,13 +1929,13 @@
         <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1888,13 +1943,13 @@
         <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1902,7 +1957,7 @@
         <v>35</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
@@ -1916,7 +1971,7 @@
         <v>37</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D17" t="s">
         <v>38</v>
@@ -1930,7 +1985,7 @@
         <v>40</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D18" t="s">
         <v>41</v>
@@ -1944,7 +1999,7 @@
         <v>43</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -1958,7 +2013,7 @@
         <v>45</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
@@ -1972,7 +2027,7 @@
         <v>47</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
@@ -1986,7 +2041,7 @@
         <v>49</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
@@ -2000,7 +2055,7 @@
         <v>51</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D23" t="s">
         <v>41</v>
@@ -2014,7 +2069,7 @@
         <v>53</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D24" t="s">
         <v>22</v>
@@ -2028,7 +2083,7 @@
         <v>16</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
@@ -2042,7 +2097,7 @@
         <v>56</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
@@ -2056,7 +2111,7 @@
         <v>58</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D27" t="s">
         <v>14</v>
@@ -2070,7 +2125,7 @@
         <v>60</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
@@ -2084,7 +2139,7 @@
         <v>16</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D29" t="s">
         <v>17</v>
@@ -2098,7 +2153,7 @@
         <v>16</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D30" t="s">
         <v>17</v>
@@ -2112,7 +2167,7 @@
         <v>64</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D31" t="s">
         <v>17</v>
@@ -2126,7 +2181,7 @@
         <v>66</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D32" t="s">
         <v>14</v>
@@ -2140,7 +2195,7 @@
         <v>67</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D33" t="s">
         <v>14</v>
@@ -2154,7 +2209,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
@@ -2168,7 +2223,7 @@
         <v>70</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
@@ -2182,7 +2237,7 @@
         <v>72</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -2196,7 +2251,7 @@
         <v>74</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D37" t="s">
         <v>27</v>
@@ -2210,7 +2265,7 @@
         <v>76</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D38" t="s">
         <v>41</v>
@@ -2224,7 +2279,7 @@
         <v>78</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D39" t="s">
         <v>5</v>
@@ -2238,7 +2293,7 @@
         <v>80</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D40" t="s">
         <v>27</v>
@@ -2252,7 +2307,7 @@
         <v>82</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D41" t="s">
         <v>41</v>
@@ -2266,7 +2321,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D42" t="s">
         <v>14</v>
@@ -2280,7 +2335,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D43" t="s">
         <v>5</v>
@@ -2294,7 +2349,7 @@
         <v>16</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D44" t="s">
         <v>17</v>
@@ -2308,7 +2363,7 @@
         <v>16</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D45" t="s">
         <v>17</v>
@@ -2322,7 +2377,7 @@
         <v>90</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D46" t="s">
         <v>10</v>
@@ -2336,7 +2391,7 @@
         <v>92</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D47" t="s">
         <v>10</v>
@@ -2350,7 +2405,7 @@
         <v>94</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D48" t="s">
         <v>41</v>
@@ -2364,7 +2419,7 @@
         <v>96</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D49" t="s">
         <v>5</v>
@@ -2378,7 +2433,7 @@
         <v>98</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D50" t="s">
         <v>14</v>
@@ -2392,7 +2447,7 @@
         <v>100</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D51" t="s">
         <v>5</v>
@@ -2406,7 +2461,7 @@
         <v>102</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D52" t="s">
         <v>38</v>
@@ -2420,7 +2475,7 @@
         <v>104</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D53" t="s">
         <v>17</v>
@@ -2434,7 +2489,7 @@
         <v>106</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D54" t="s">
         <v>22</v>
@@ -2448,7 +2503,7 @@
         <v>16</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D55" t="s">
         <v>17</v>
@@ -2462,7 +2517,7 @@
         <v>109</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D56" t="s">
         <v>27</v>
@@ -2476,7 +2531,7 @@
         <v>111</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D57" t="s">
         <v>27</v>
@@ -2490,7 +2545,7 @@
         <v>113</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D58" t="s">
         <v>10</v>
@@ -2504,7 +2559,7 @@
         <v>115</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D59" t="s">
         <v>41</v>
@@ -2518,7 +2573,7 @@
         <v>16</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D60" t="s">
         <v>17</v>
@@ -2532,7 +2587,7 @@
         <v>118</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D61" t="s">
         <v>38</v>
@@ -2546,7 +2601,7 @@
         <v>16</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D62" t="s">
         <v>17</v>
@@ -2560,7 +2615,7 @@
         <v>16</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D63" t="s">
         <v>17</v>
@@ -2574,231 +2629,238 @@
         <v>122</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D64" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>123</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>124</v>
+        <v>417</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D65" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E65" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D66" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>125</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="C67" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D67" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>127</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="C68" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D68" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>129</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="C69" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D69" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D70" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D71" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>133</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="C72" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D72" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="73" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="C73" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="C74" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>136</v>
-      </c>
-      <c r="B74" s="2" t="s">
+      <c r="E74" s="5"/>
+    </row>
+    <row r="75" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>138</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="D74" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>139</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D75" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>139</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="C76" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D76" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>141</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="C77" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D77" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>143</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="C78" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D78" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>145</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="C79" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D79" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>147</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="C80" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D80" t="s">
         <v>14</v>
@@ -2806,13 +2868,13 @@
     </row>
     <row r="81" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>149</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="C81" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D81" t="s">
         <v>5</v>
@@ -2820,13 +2882,13 @@
     </row>
     <row r="82" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>151</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="C82" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D82" t="s">
         <v>10</v>
@@ -2834,13 +2896,13 @@
     </row>
     <row r="83" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>153</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="C83" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D83" t="s">
         <v>27</v>
@@ -2848,13 +2910,13 @@
     </row>
     <row r="84" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>155</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="C84" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D84" t="s">
         <v>22</v>
@@ -2862,13 +2924,13 @@
     </row>
     <row r="85" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>157</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="C85" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D85" t="s">
         <v>10</v>
@@ -2876,13 +2938,13 @@
     </row>
     <row r="86" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>159</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="C86" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D86" t="s">
         <v>27</v>
@@ -2890,13 +2952,13 @@
     </row>
     <row r="87" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>161</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="C87" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D87" t="s">
         <v>10</v>
@@ -2904,13 +2966,13 @@
     </row>
     <row r="88" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D88" t="s">
         <v>17</v>
@@ -2918,13 +2980,13 @@
     </row>
     <row r="89" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>164</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="C89" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D89" t="s">
         <v>22</v>
@@ -2932,13 +2994,13 @@
     </row>
     <row r="90" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>166</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="C90" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D90" t="s">
         <v>41</v>
@@ -2946,13 +3008,13 @@
     </row>
     <row r="91" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>168</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="C91" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D91" t="s">
         <v>10</v>
@@ -2960,13 +3022,13 @@
     </row>
     <row r="92" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>170</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="C92" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D92" t="s">
         <v>17</v>
@@ -2974,13 +3036,13 @@
     </row>
     <row r="93" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D93" t="s">
         <v>17</v>
@@ -2988,13 +3050,13 @@
     </row>
     <row r="94" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>173</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="C94" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D94" t="s">
         <v>22</v>
@@ -3002,13 +3064,13 @@
     </row>
     <row r="95" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>175</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="C95" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D95" t="s">
         <v>5</v>
@@ -3016,13 +3078,13 @@
     </row>
     <row r="96" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>177</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>179</v>
-      </c>
       <c r="C96" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D96" t="s">
         <v>10</v>
@@ -3030,13 +3092,13 @@
     </row>
     <row r="97" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>179</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B97" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="C97" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D97" t="s">
         <v>27</v>
@@ -3044,13 +3106,13 @@
     </row>
     <row r="98" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>181</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B98" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="C98" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D98" t="s">
         <v>10</v>
@@ -3058,13 +3120,13 @@
     </row>
     <row r="99" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D99" t="s">
         <v>17</v>
@@ -3072,13 +3134,13 @@
     </row>
     <row r="100" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D100" t="s">
         <v>17</v>
@@ -3086,13 +3148,13 @@
     </row>
     <row r="101" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D101" t="s">
         <v>17</v>
@@ -3100,13 +3162,13 @@
     </row>
     <row r="102" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>186</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B102" s="2" t="s">
-        <v>188</v>
-      </c>
       <c r="C102" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D102" t="s">
         <v>27</v>
@@ -3114,13 +3176,13 @@
     </row>
     <row r="103" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>188</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="C103" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D103" t="s">
         <v>5</v>
@@ -3128,13 +3190,13 @@
     </row>
     <row r="104" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>190</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="C104" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D104" t="s">
         <v>41</v>
@@ -3142,13 +3204,13 @@
     </row>
     <row r="105" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D105" t="s">
         <v>17</v>
@@ -3156,13 +3218,13 @@
     </row>
     <row r="106" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D106" t="s">
         <v>17</v>
@@ -3170,13 +3232,13 @@
     </row>
     <row r="107" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>194</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B107" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="C107" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D107" t="s">
         <v>41</v>
@@ -3184,13 +3246,13 @@
     </row>
     <row r="108" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>196</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B108" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="C108" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D108" t="s">
         <v>14</v>
@@ -3198,13 +3260,13 @@
     </row>
     <row r="109" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D109" t="s">
         <v>17</v>
@@ -3212,13 +3274,13 @@
     </row>
     <row r="110" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>199</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="C110" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D110" t="s">
         <v>27</v>
@@ -3226,13 +3288,13 @@
     </row>
     <row r="111" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>201</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B111" s="2" t="s">
-        <v>203</v>
-      </c>
       <c r="C111" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D111" t="s">
         <v>10</v>
@@ -3240,13 +3302,13 @@
     </row>
     <row r="112" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D112" t="s">
         <v>10</v>
@@ -3254,13 +3316,13 @@
     </row>
     <row r="113" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D113" t="s">
         <v>17</v>
@@ -3268,13 +3330,13 @@
     </row>
     <row r="114" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
+        <v>205</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B114" s="2" t="s">
-        <v>207</v>
-      </c>
       <c r="C114" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D114" t="s">
         <v>41</v>
@@ -3282,13 +3344,13 @@
     </row>
     <row r="115" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
+        <v>207</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B115" s="2" t="s">
-        <v>209</v>
-      </c>
       <c r="C115" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D115" t="s">
         <v>41</v>
@@ -3296,13 +3358,13 @@
     </row>
     <row r="116" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D116" t="s">
         <v>17</v>
@@ -3310,13 +3372,13 @@
     </row>
     <row r="117" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>210</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B117" s="2" t="s">
-        <v>212</v>
-      </c>
       <c r="C117" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D117" t="s">
         <v>5</v>
@@ -3324,13 +3386,13 @@
     </row>
     <row r="118" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D118" t="s">
         <v>5</v>
@@ -3338,13 +3400,13 @@
     </row>
     <row r="119" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>213</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B119" s="2" t="s">
-        <v>215</v>
-      </c>
       <c r="C119" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D119" t="s">
         <v>27</v>
@@ -3352,13 +3414,13 @@
     </row>
     <row r="120" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D120" t="s">
         <v>17</v>
@@ -3366,13 +3428,13 @@
     </row>
     <row r="121" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
+        <v>216</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B121" s="2" t="s">
-        <v>218</v>
-      </c>
       <c r="C121" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D121" t="s">
         <v>10</v>
@@ -3380,13 +3442,13 @@
     </row>
     <row r="122" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D122" t="s">
         <v>10</v>
@@ -3394,13 +3456,13 @@
     </row>
     <row r="123" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
+        <v>219</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B123" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="C123" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D123" t="s">
         <v>10</v>
@@ -3408,13 +3470,13 @@
     </row>
     <row r="124" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
+        <v>221</v>
+      </c>
+      <c r="B124" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B124" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="C124" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D124" t="s">
         <v>27</v>
@@ -3422,13 +3484,13 @@
     </row>
     <row r="125" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D125" t="s">
         <v>17</v>
@@ -3436,27 +3498,27 @@
     </row>
     <row r="126" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>224</v>
+      </c>
+      <c r="B126" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="C126" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D126" t="s">
         <v>226</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="D126" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
+        <v>227</v>
+      </c>
+      <c r="B127" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B127" s="2" t="s">
-        <v>229</v>
-      </c>
       <c r="C127" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D127" t="s">
         <v>5</v>
@@ -3464,13 +3526,13 @@
     </row>
     <row r="128" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D128" t="s">
         <v>17</v>
@@ -3478,13 +3540,13 @@
     </row>
     <row r="129" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D129" t="s">
         <v>10</v>
@@ -3492,13 +3554,13 @@
     </row>
     <row r="130" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
+        <v>231</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B130" s="2" t="s">
-        <v>233</v>
-      </c>
       <c r="C130" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D130" t="s">
         <v>27</v>
@@ -3506,13 +3568,13 @@
     </row>
     <row r="131" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
+        <v>233</v>
+      </c>
+      <c r="B131" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B131" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="C131" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D131" t="s">
         <v>17</v>
@@ -3520,13 +3582,13 @@
     </row>
     <row r="132" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
+        <v>235</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B132" s="2" t="s">
-        <v>237</v>
-      </c>
       <c r="C132" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D132" t="s">
         <v>10</v>
@@ -3534,13 +3596,13 @@
     </row>
     <row r="133" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
+        <v>237</v>
+      </c>
+      <c r="B133" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>239</v>
-      </c>
       <c r="C133" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D133" t="s">
         <v>22</v>
@@ -3548,13 +3610,13 @@
     </row>
     <row r="134" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>239</v>
+      </c>
+      <c r="B134" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B134" s="2" t="s">
-        <v>241</v>
-      </c>
       <c r="C134" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D134" t="s">
         <v>41</v>
@@ -3562,13 +3624,13 @@
     </row>
     <row r="135" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
+        <v>241</v>
+      </c>
+      <c r="B135" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B135" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="C135" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D135" t="s">
         <v>10</v>
@@ -3576,13 +3638,13 @@
     </row>
     <row r="136" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
+        <v>243</v>
+      </c>
+      <c r="B136" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B136" s="2" t="s">
-        <v>245</v>
-      </c>
       <c r="C136" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D136" t="s">
         <v>41</v>
@@ -3590,13 +3652,13 @@
     </row>
     <row r="137" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
+        <v>245</v>
+      </c>
+      <c r="B137" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B137" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="C137" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D137" t="s">
         <v>41</v>
@@ -3604,13 +3666,13 @@
     </row>
     <row r="138" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D138" t="s">
         <v>41</v>
@@ -3618,13 +3680,13 @@
     </row>
     <row r="139" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
+        <v>248</v>
+      </c>
+      <c r="B139" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="B139" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="C139" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D139" t="s">
         <v>17</v>
@@ -3632,13 +3694,13 @@
     </row>
     <row r="140" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
+        <v>250</v>
+      </c>
+      <c r="B140" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B140" s="2" t="s">
-        <v>252</v>
-      </c>
       <c r="C140" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D140" t="s">
         <v>22</v>
@@ -3646,13 +3708,13 @@
     </row>
     <row r="141" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
+        <v>252</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B141" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="C141" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D141" t="s">
         <v>10</v>
@@ -3660,13 +3722,13 @@
     </row>
     <row r="142" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D142" t="s">
         <v>10</v>
@@ -3674,13 +3736,13 @@
     </row>
     <row r="143" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
+        <v>255</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B143" s="2" t="s">
-        <v>257</v>
-      </c>
       <c r="C143" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D143" t="s">
         <v>10</v>
@@ -3688,13 +3750,13 @@
     </row>
     <row r="144" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
+        <v>257</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B144" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="C144" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D144" t="s">
         <v>5</v>
@@ -3702,13 +3764,13 @@
     </row>
     <row r="145" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
+        <v>259</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B145" s="2" t="s">
-        <v>261</v>
-      </c>
       <c r="C145" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D145" t="s">
         <v>22</v>
@@ -3716,13 +3778,13 @@
     </row>
     <row r="146" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
+        <v>261</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B146" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="C146" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D146" t="s">
         <v>10</v>
@@ -3730,13 +3792,13 @@
     </row>
     <row r="147" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
+        <v>263</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B147" s="2" t="s">
-        <v>265</v>
-      </c>
       <c r="C147" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D147" t="s">
         <v>10</v>
@@ -3744,13 +3806,13 @@
     </row>
     <row r="148" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
+        <v>265</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="B148" s="2" t="s">
-        <v>267</v>
-      </c>
       <c r="C148" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D148" t="s">
         <v>22</v>
@@ -3758,13 +3820,13 @@
     </row>
     <row r="149" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
+        <v>267</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B149" s="2" t="s">
-        <v>269</v>
-      </c>
       <c r="C149" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D149" t="s">
         <v>10</v>
@@ -3772,13 +3834,13 @@
     </row>
     <row r="150" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
+        <v>269</v>
+      </c>
+      <c r="B150" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B150" s="2" t="s">
-        <v>271</v>
-      </c>
       <c r="C150" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D150" t="s">
         <v>27</v>
@@ -3786,13 +3848,13 @@
     </row>
     <row r="151" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D151" t="s">
         <v>17</v>
@@ -3800,13 +3862,13 @@
     </row>
     <row r="152" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
+        <v>272</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B152" s="2" t="s">
-        <v>274</v>
-      </c>
       <c r="C152" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D152" t="s">
         <v>10</v>
@@ -3814,27 +3876,27 @@
     </row>
     <row r="153" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
+        <v>274</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="C153" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D153" t="s">
         <v>276</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="D153" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
+        <v>277</v>
+      </c>
+      <c r="B154" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B154" s="2" t="s">
-        <v>279</v>
-      </c>
       <c r="C154" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D154" t="s">
         <v>41</v>
@@ -3842,13 +3904,13 @@
     </row>
     <row r="155" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
+        <v>279</v>
+      </c>
+      <c r="B155" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B155" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="C155" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D155" t="s">
         <v>10</v>
@@ -3856,13 +3918,13 @@
     </row>
     <row r="156" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D156" t="s">
         <v>17</v>
@@ -3870,27 +3932,27 @@
     </row>
     <row r="157" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
+        <v>282</v>
+      </c>
+      <c r="B157" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B157" s="2" t="s">
-        <v>284</v>
-      </c>
       <c r="C157" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D157" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
+        <v>284</v>
+      </c>
+      <c r="B158" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B158" s="2" t="s">
-        <v>286</v>
-      </c>
       <c r="C158" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D158" t="s">
         <v>10</v>
@@ -3898,13 +3960,13 @@
     </row>
     <row r="159" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
+        <v>286</v>
+      </c>
+      <c r="B159" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B159" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="C159" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D159" t="s">
         <v>5</v>
@@ -3912,13 +3974,13 @@
     </row>
     <row r="160" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>288</v>
+      </c>
+      <c r="B160" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="B160" s="2" t="s">
-        <v>290</v>
-      </c>
       <c r="C160" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D160" t="s">
         <v>27</v>
@@ -3926,13 +3988,13 @@
     </row>
     <row r="161" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
+        <v>290</v>
+      </c>
+      <c r="B161" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B161" s="2" t="s">
-        <v>292</v>
-      </c>
       <c r="C161" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D161" t="s">
         <v>5</v>
@@ -3940,13 +4002,13 @@
     </row>
     <row r="162" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D162" t="s">
         <v>5</v>
@@ -3954,13 +4016,13 @@
     </row>
     <row r="163" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
+        <v>293</v>
+      </c>
+      <c r="B163" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B163" s="2" t="s">
-        <v>295</v>
-      </c>
       <c r="C163" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D163" t="s">
         <v>22</v>
@@ -3968,13 +4030,13 @@
     </row>
     <row r="164" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
+        <v>295</v>
+      </c>
+      <c r="B164" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B164" s="2" t="s">
-        <v>297</v>
-      </c>
       <c r="C164" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D164" t="s">
         <v>38</v>
@@ -3982,13 +4044,13 @@
     </row>
     <row r="165" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
+        <v>297</v>
+      </c>
+      <c r="B165" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B165" s="2" t="s">
-        <v>299</v>
-      </c>
       <c r="C165" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D165" t="s">
         <v>22</v>
@@ -3996,13 +4058,13 @@
     </row>
     <row r="166" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
+        <v>299</v>
+      </c>
+      <c r="B166" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B166" s="2" t="s">
-        <v>301</v>
-      </c>
       <c r="C166" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D166" t="s">
         <v>27</v>
@@ -4010,13 +4072,13 @@
     </row>
     <row r="167" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
+        <v>301</v>
+      </c>
+      <c r="B167" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B167" s="2" t="s">
-        <v>303</v>
-      </c>
       <c r="C167" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D167" t="s">
         <v>22</v>
@@ -4024,13 +4086,13 @@
     </row>
     <row r="168" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
+        <v>303</v>
+      </c>
+      <c r="B168" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B168" s="2" t="s">
-        <v>305</v>
-      </c>
       <c r="C168" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D168" t="s">
         <v>27</v>
@@ -4038,13 +4100,13 @@
     </row>
     <row r="169" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
+        <v>305</v>
+      </c>
+      <c r="B169" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="B169" s="2" t="s">
-        <v>307</v>
-      </c>
       <c r="C169" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D169" t="s">
         <v>2</v>
@@ -4052,13 +4114,13 @@
     </row>
     <row r="170" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
+        <v>307</v>
+      </c>
+      <c r="B170" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B170" s="2" t="s">
-        <v>309</v>
-      </c>
       <c r="C170" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D170" t="s">
         <v>5</v>
@@ -4066,13 +4128,13 @@
     </row>
     <row r="171" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
+        <v>309</v>
+      </c>
+      <c r="B171" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B171" s="2" t="s">
-        <v>311</v>
-      </c>
       <c r="C171" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D171" t="s">
         <v>22</v>
@@ -4080,13 +4142,13 @@
     </row>
     <row r="172" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
+        <v>311</v>
+      </c>
+      <c r="B172" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="B172" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="C172" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D172" t="s">
         <v>5</v>
@@ -4094,13 +4156,13 @@
     </row>
     <row r="173" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
+        <v>313</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B173" s="2" t="s">
-        <v>315</v>
-      </c>
       <c r="C173" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D173" t="s">
         <v>5</v>
@@ -4108,13 +4170,13 @@
     </row>
     <row r="174" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
+        <v>315</v>
+      </c>
+      <c r="B174" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="B174" s="2" t="s">
-        <v>317</v>
-      </c>
       <c r="C174" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D174" t="s">
         <v>41</v>
@@ -4122,13 +4184,13 @@
     </row>
     <row r="175" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
+        <v>317</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="B175" s="2" t="s">
-        <v>319</v>
-      </c>
       <c r="C175" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D175" t="s">
         <v>41</v>
@@ -4136,13 +4198,13 @@
     </row>
     <row r="176" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
+        <v>319</v>
+      </c>
+      <c r="B176" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B176" s="2" t="s">
-        <v>321</v>
-      </c>
       <c r="C176" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D176" t="s">
         <v>10</v>
@@ -4150,27 +4212,27 @@
     </row>
     <row r="177" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
+        <v>321</v>
+      </c>
+      <c r="B177" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B177" s="2" t="s">
-        <v>323</v>
-      </c>
       <c r="C177" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D177" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
+        <v>323</v>
+      </c>
+      <c r="B178" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B178" s="2" t="s">
-        <v>325</v>
-      </c>
       <c r="C178" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D178" t="s">
         <v>22</v>
@@ -4178,13 +4240,13 @@
     </row>
     <row r="179" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D179" t="s">
         <v>17</v>
@@ -4192,13 +4254,13 @@
     </row>
     <row r="180" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D180" t="s">
         <v>17</v>
@@ -4206,13 +4268,13 @@
     </row>
     <row r="181" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
+        <v>327</v>
+      </c>
+      <c r="B181" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B181" s="2" t="s">
-        <v>329</v>
-      </c>
       <c r="C181" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D181" t="s">
         <v>22</v>
@@ -4220,13 +4282,13 @@
     </row>
     <row r="182" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B182" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D182" t="s">
         <v>17</v>
@@ -4234,13 +4296,13 @@
     </row>
     <row r="183" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
+        <v>330</v>
+      </c>
+      <c r="B183" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B183" s="2" t="s">
-        <v>332</v>
-      </c>
       <c r="C183" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D183" t="s">
         <v>5</v>
@@ -4248,13 +4310,13 @@
     </row>
     <row r="184" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B184" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D184" t="s">
         <v>17</v>
@@ -4262,13 +4324,13 @@
     </row>
     <row r="185" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
+        <v>333</v>
+      </c>
+      <c r="B185" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="B185" s="2" t="s">
-        <v>335</v>
-      </c>
       <c r="C185" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D185" t="s">
         <v>10</v>
@@ -4276,13 +4338,13 @@
     </row>
     <row r="186" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
+        <v>335</v>
+      </c>
+      <c r="B186" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B186" s="2" t="s">
-        <v>337</v>
-      </c>
       <c r="C186" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D186" t="s">
         <v>27</v>
@@ -4290,13 +4352,13 @@
     </row>
     <row r="187" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
+        <v>337</v>
+      </c>
+      <c r="B187" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B187" s="2" t="s">
-        <v>339</v>
-      </c>
       <c r="C187" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D187" t="s">
         <v>5</v>
@@ -4304,13 +4366,13 @@
     </row>
     <row r="188" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
+        <v>339</v>
+      </c>
+      <c r="B188" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B188" s="2" t="s">
-        <v>341</v>
-      </c>
       <c r="C188" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D188" t="s">
         <v>17</v>
@@ -4318,13 +4380,13 @@
     </row>
     <row r="189" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
+        <v>341</v>
+      </c>
+      <c r="B189" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B189" s="2" t="s">
-        <v>343</v>
-      </c>
       <c r="C189" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D189" t="s">
         <v>5</v>
@@ -4332,13 +4394,13 @@
     </row>
     <row r="190" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D190" t="s">
         <v>17</v>
@@ -4346,13 +4408,13 @@
     </row>
     <row r="191" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
+        <v>344</v>
+      </c>
+      <c r="B191" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B191" s="2" t="s">
-        <v>346</v>
-      </c>
       <c r="C191" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D191" t="s">
         <v>41</v>
@@ -4360,237 +4422,243 @@
     </row>
     <row r="192" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B192" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D192" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
+        <v>347</v>
+      </c>
+      <c r="B193" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B193" s="2" t="s">
-        <v>349</v>
-      </c>
       <c r="C193" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D193" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
+        <v>349</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="B194" s="2" t="s">
-        <v>351</v>
-      </c>
       <c r="C194" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D194" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
+        <v>351</v>
+      </c>
+      <c r="B195" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="B195" s="2" t="s">
-        <v>353</v>
-      </c>
       <c r="C195" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D195" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
+        <v>353</v>
+      </c>
+      <c r="B196" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B196" s="2" t="s">
-        <v>355</v>
-      </c>
       <c r="C196" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D196" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
+        <v>355</v>
+      </c>
+      <c r="B197" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="B197" s="2" t="s">
-        <v>357</v>
-      </c>
       <c r="C197" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D197" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A198" t="s">
+    <row r="198" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A198" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="B198" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="C198" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="D198" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E198" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="F198" s="6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
         <v>358</v>
       </c>
-      <c r="B198" s="2" t="s">
+      <c r="B199" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="C198" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="D198" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A199" t="s">
-        <v>360</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>361</v>
-      </c>
       <c r="C199" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D199" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D200" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B201" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D201" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D202" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D203" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D204" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D205" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D206" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D207" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B208" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D208" t="s">
         <v>17</v>
@@ -4598,27 +4666,27 @@
     </row>
     <row r="209" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D209" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D210" t="s">
         <v>22</v>
@@ -4626,13 +4694,13 @@
     </row>
     <row r="211" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D211" t="s">
         <v>10</v>
@@ -4640,13 +4708,13 @@
     </row>
     <row r="212" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D212" t="s">
         <v>27</v>
@@ -4654,13 +4722,13 @@
     </row>
     <row r="213" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D213" t="s">
         <v>5</v>
@@ -4668,13 +4736,13 @@
     </row>
     <row r="214" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D214" t="s">
         <v>41</v>
@@ -4682,13 +4750,13 @@
     </row>
     <row r="215" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D215" t="s">
         <v>17</v>
@@ -4696,13 +4764,13 @@
     </row>
     <row r="216" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D216" t="s">
         <v>2</v>
@@ -4710,13 +4778,13 @@
     </row>
     <row r="217" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D217" t="s">
         <v>41</v>
@@ -4724,13 +4792,13 @@
     </row>
     <row r="218" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D218" t="s">
         <v>41</v>
@@ -4738,13 +4806,13 @@
     </row>
     <row r="219" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D219" t="s">
         <v>41</v>
@@ -4752,13 +4820,13 @@
     </row>
     <row r="220" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B220" s="2" t="s">
         <v>109</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D220" t="s">
         <v>27</v>
@@ -4766,13 +4834,13 @@
     </row>
     <row r="221" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D221" t="s">
         <v>10</v>
@@ -4780,13 +4848,13 @@
     </row>
     <row r="222" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D222" t="s">
         <v>41</v>
@@ -4794,13 +4862,13 @@
     </row>
     <row r="223" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D223" t="s">
         <v>22</v>
@@ -4808,13 +4876,13 @@
     </row>
     <row r="224" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D224" t="s">
         <v>17</v>
@@ -4822,13 +4890,13 @@
     </row>
     <row r="225" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B225" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D225" t="s">
         <v>17</v>
@@ -4836,13 +4904,13 @@
     </row>
     <row r="226" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D226" t="s">
         <v>5</v>
@@ -4850,33 +4918,36 @@
     </row>
     <row r="227" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D227" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B228" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D228" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E73:E74"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More info about Allen Street.
</commit_message>
<xml_diff>
--- a/Master Info.xlsx
+++ b/Master Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryansmith/Documents/Coding/topomapper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3BD399-EECF-704D-89DB-01C6552E42A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEE406E-FC2F-1344-93D6-F85D484FFDB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38420" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{1807FE50-C9A7-E24A-AB34-CDD2C78B0884}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="427">
   <si>
     <t xml:space="preserve">Alexandra Street </t>
   </si>
@@ -63,9 +63,6 @@
     <t xml:space="preserve">Allen Street </t>
   </si>
   <si>
-    <t xml:space="preserve"> Named for Samuel Allen, a businessperson and owner of a produce store on Flinders and a hotel. He later became an Alderman as well. (Mathew, 2008, p. 7). </t>
-  </si>
-  <si>
     <t xml:space="preserve"> business</t>
   </si>
   <si>
@@ -1317,13 +1314,25 @@
     <t>Named for Captain Charles Sturt, one time Surveyor General of South Australia (Mathew, 2008, p. 115). A well traveled explorer, Sturt made many journeys inland, helping to map the interior. During one such journey, Dowling (2017) argues, Sturt noticed the spread of syphilis, one of the sexually transmitted STIs brought over by Europeans. To learn more, consider Sturt's writings about two expeditions inland: &lt;a href='https://books.google.com.au/books?hl=en&amp;lr=&amp;id=nMDCDwAAQBAJ&amp;oi=fnd&amp;pg=PT8&amp;dq=charles+sturt&amp;ots=l9oaADIRFt&amp;sig=Uc2JuFkj7Wb678CM-3tQJ-mATAw&amp;redir_esc=y#v=onepage&amp;q=charles%20sturt&amp;f=false'&gt;source&lt;/a&gt;.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Named for "Alexandra of Denmark (1844-1925) [who] married Albert Edward (later Edward VII), the eldest son of Queen Victoria in 1863" (Mathew, 2008, p. 6). "A most indefatigable letter-writer" for whom "thirty or forty letters from her pen is no unusual daily occurrence" ("Queen Alexandra", 1903, p. 39), Alexandra was widely loved, with one newspaper article written about her, reporting that "her conduct and deportment were admirable in every way," a description that was argued to have echoed Charles Dickens's own description of her ("QUEEN ALEXANDRA", 1913, p. 6). Alexandra also partook in photography as a craft, producing albums with designs and watercolours including one of collages produced in c. 1866-1869 (Royal Collection Trust, n.d).</t>
-  </si>
-  <si>
     <t>Mathew, J. (2008). &lt;i&gt;Highways and Byways: The Origin of Townsville Street Names&lt;/i&gt; (Revised ed.). Townsville, QLD: Townsville Library Service.&lt;p&gt;&lt;/p&gt;Queen Alexandra. (1903, Sept 11). &lt;i&gt;The Week&lt;/i&gt;, p. 39.&lt;p&gt;&lt;/p&gt;QUEEN ALEXANDRA. (1913, Mar 11). &lt;i&gt;The Register&lt;/i&gt;, p. 6.&lt;p&gt;&lt;/p&gt;Royal Collection Trust. (n.d.). &lt;i&gt;Album of designs, incorporating photographs c.1866-9&lt;/i&gt;. Retrieved from &lt;a href='https://www.rct.uk/collection/2300089/album-of-designs-incorporating-photographs#/referer/233758/creator'&gt;https://www.rct.uk/collection/2300089/album-of-designs-incorporating-photographs#/referer/233758/creator&lt;/a&gt;.</t>
   </si>
   <si>
     <t>Updated in App</t>
+  </si>
+  <si>
+    <t>HEAVY GALE AND FLOODS IN THE NORTH. (1884, Feb 29). &lt;i&gt;The Brisbane Courier&lt;/i&gt;, p. 5.&lt;p&gt;&lt;/p&gt;Mathew, J. (2008). &lt;i&gt;Highways and Byways: The Origin of Townsville Street Names&lt;/i&gt; (Revised ed.). Townsville, QLD: Townsville Library Service.&lt;p&gt;&lt;/p&gt;Queensland Government. (2022). &lt;i&gt;Samuel Allen &amp; Sons (former)&lt;/i&gt;. Retrieved from &lt;a href=\"https://apps.des.qld.gov.au/heritage-register/detail/?id=600903\"&gt;https://apps.des.qld.gov.au/heritage-register/detail/?id=600903&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Named for Samuel Allen, a businessperson and owner of a produce store on Flinders and a hotel. He later became an Alderman as well. (Mathew, 2008, p. 7). During a flood in 1884, Allen was impacted heavily, with one report in &lt;i&gt;The Brisbane Courier&lt;/i&gt; describing the loss thusly: \"a large and valuable stock of various kinds of agricultural produce—burst out through the street entrance and carried bags of maize and kegs of butter down the street,\" the result of which was the paper simply concluding that he was \"a heavy loser\" in the floods (\"HEAVY GALE AND FLOODS IN THE NORTH\", 1884, p. 5). A building owned by Allen at 247 Flinders Street is now listed on the Queensland Heritage Register (Queensland Government, 2022).B2:B3</t>
+  </si>
+  <si>
+    <t>Named for "Alexandra of Denmark (1844-1925) [who] married Albert Edward (later Edward VII), the eldest son of Queen Victoria in 1863" (Mathew, 2008, p. 6). "A most indefatigable letter-writer" for whom "thirty or forty letters from her pen is no unusual daily occurrence" ("Queen Alexandra", 1903, p. 39), Alexandra was widely loved, with one newspaper article written about her, reporting that "her conduct and deportment were admirable in every way," a description that was argued to have echoed Charles Dickens's own description of her ("QUEEN ALEXANDRA", 1913, p. 6). Alexandra also partook in photography as a craft, producing albums with designs and watercolours including one of collages produced in c. 1866-1869 (Royal Collection Trust, n.d).</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>JCU Library has Special Collections material for the company: https://libserver.jcu.edu.au/specials/Archives/samuelallen.html</t>
   </si>
 </sst>
 </file>
@@ -1707,12 +1716,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC5444A-5FE5-E14D-8DB4-EE518C4047AC}">
-  <dimension ref="A1:F227"/>
+  <dimension ref="A1:G227"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="760" activePane="bottomLeft"/>
       <selection activeCell="E199" sqref="E199"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1722,2370 +1731,2380 @@
     <col min="3" max="3" width="100.1640625" customWidth="1"/>
     <col min="5" max="5" width="43.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="106.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>411</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>415</v>
+      </c>
+      <c r="G3" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D17" t="s">
         <v>36</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D18" t="s">
         <v>39</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D18" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="C21" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="C23" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D25" t="s">
         <v>15</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D25" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D29" t="s">
         <v>15</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D29" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D30" t="s">
         <v>15</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D30" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="C31" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C32" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C34" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="C36" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="C37" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="C38" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="C39" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D39" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="C40" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="C41" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="C42" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="C43" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D43" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D44" t="s">
         <v>15</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D44" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D45" t="s">
         <v>15</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D45" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="C46" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="C47" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="C48" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="C49" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D49" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="C50" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>97</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="C51" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D51" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="C52" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D52" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="C53" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="C54" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D55" t="s">
         <v>15</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D55" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>106</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="C56" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D56" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>108</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="C57" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D57" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="C58" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="C59" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D59" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D60" t="s">
         <v>15</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D60" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>115</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="C61" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D62" t="s">
         <v>15</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D62" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D63" t="s">
         <v>15</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D63" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="C64" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D64" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D65" t="s">
+        <v>39</v>
+      </c>
+      <c r="E65" t="s">
         <v>415</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="D65" t="s">
-        <v>40</v>
-      </c>
-      <c r="E65" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D66" t="s">
         <v>15</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D66" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>123</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="C67" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D67" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>125</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="C68" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>127</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="C69" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D69" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D70" t="s">
         <v>15</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D70" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D71" t="s">
         <v>15</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D71" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>131</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="C72" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>133</v>
+      </c>
+      <c r="B73" t="s">
         <v>134</v>
       </c>
-      <c r="B73" t="s">
-        <v>135</v>
-      </c>
       <c r="C73" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D73" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D74" t="s">
         <v>15</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D74" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>136</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="C75" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D75" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>138</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="C76" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>140</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="C77" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D77" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>142</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="C78" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D78" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>144</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="C79" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D79" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>146</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="C80" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D80" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>148</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="C81" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D81" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>150</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="C82" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D82" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>152</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="C83" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D83" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>154</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>156</v>
-      </c>
       <c r="C84" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D84" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>156</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="C85" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D85" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>158</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="C86" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D86" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D87" t="s">
         <v>15</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D87" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>161</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="C88" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D88" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>163</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="C89" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D89" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>165</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="C90" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D90" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>167</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="C91" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D91" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B92" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D92" t="s">
         <v>15</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D92" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>170</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B93" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="C93" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D93" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>172</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="C94" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D94" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>174</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>176</v>
-      </c>
       <c r="C95" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D95" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>176</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>178</v>
-      </c>
       <c r="C96" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D96" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>178</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B97" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="C97" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D97" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B98" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D98" t="s">
         <v>15</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D98" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B99" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D99" t="s">
         <v>15</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D99" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B100" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D100" t="s">
         <v>15</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D100" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>183</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B101" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="C101" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D101" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>185</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B102" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="C102" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D102" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>187</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="C103" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D103" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B104" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D104" t="s">
         <v>15</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D104" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B105" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D105" t="s">
         <v>15</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D105" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>191</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B106" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="C106" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D106" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>193</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B107" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="C107" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D107" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B108" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D108" t="s">
         <v>15</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D108" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>196</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B109" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="C109" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D109" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>198</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>200</v>
-      </c>
       <c r="C110" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D110" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D111" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B112" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D112" t="s">
         <v>15</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D112" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
+        <v>202</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="C113" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D113" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
+        <v>204</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B114" s="2" t="s">
-        <v>206</v>
-      </c>
       <c r="C114" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D114" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B115" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D115" t="s">
         <v>15</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D115" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
+        <v>207</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B116" s="2" t="s">
-        <v>209</v>
-      </c>
       <c r="C116" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D116" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D117" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
+        <v>210</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B118" s="2" t="s">
-        <v>212</v>
-      </c>
       <c r="C118" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D118" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B119" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D119" t="s">
         <v>15</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D119" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
+        <v>213</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B120" s="2" t="s">
-        <v>215</v>
-      </c>
       <c r="C120" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D120" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D121" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
+        <v>216</v>
+      </c>
+      <c r="B122" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B122" s="2" t="s">
-        <v>218</v>
-      </c>
       <c r="C122" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D122" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
+        <v>218</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B123" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="C123" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D123" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B124" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D124" t="s">
         <v>15</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D124" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
+        <v>221</v>
+      </c>
+      <c r="B125" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="C125" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D125" t="s">
         <v>223</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D125" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>224</v>
+      </c>
+      <c r="B126" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B126" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="C126" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D126" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B127" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D127" t="s">
         <v>15</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D127" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D128" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
+        <v>228</v>
+      </c>
+      <c r="B129" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B129" s="2" t="s">
-        <v>230</v>
-      </c>
       <c r="C129" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D129" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
+        <v>230</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B130" s="2" t="s">
-        <v>232</v>
-      </c>
       <c r="C130" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D130" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
+        <v>232</v>
+      </c>
+      <c r="B131" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B131" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="C131" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D131" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
+        <v>234</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B132" s="2" t="s">
-        <v>236</v>
-      </c>
       <c r="C132" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D132" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
+        <v>236</v>
+      </c>
+      <c r="B133" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="C133" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D133" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>238</v>
+      </c>
+      <c r="B134" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B134" s="2" t="s">
-        <v>240</v>
-      </c>
       <c r="C134" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D134" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
+        <v>240</v>
+      </c>
+      <c r="B135" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B135" s="2" t="s">
-        <v>242</v>
-      </c>
       <c r="C135" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D135" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
+        <v>242</v>
+      </c>
+      <c r="B136" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B136" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="C136" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D136" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D137" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
+        <v>245</v>
+      </c>
+      <c r="B138" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B138" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="C138" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D138" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
+        <v>247</v>
+      </c>
+      <c r="B139" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B139" s="2" t="s">
-        <v>249</v>
-      </c>
       <c r="C139" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D139" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
+        <v>249</v>
+      </c>
+      <c r="B140" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B140" s="2" t="s">
-        <v>251</v>
-      </c>
       <c r="C140" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D140" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D141" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
+        <v>252</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B142" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="C142" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D142" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
+        <v>254</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B143" s="2" t="s">
-        <v>256</v>
-      </c>
       <c r="C143" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D143" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
+        <v>256</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B144" s="2" t="s">
-        <v>258</v>
-      </c>
       <c r="C144" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D144" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
+        <v>258</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B145" s="2" t="s">
-        <v>260</v>
-      </c>
       <c r="C145" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D145" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
+        <v>260</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B146" s="2" t="s">
-        <v>262</v>
-      </c>
       <c r="C146" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D146" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
+        <v>262</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B147" s="2" t="s">
-        <v>264</v>
-      </c>
       <c r="C147" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D147" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
+        <v>264</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B148" s="2" t="s">
-        <v>266</v>
-      </c>
       <c r="C148" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D148" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
+        <v>266</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B149" s="2" t="s">
-        <v>268</v>
-      </c>
       <c r="C149" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D149" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B150" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D150" t="s">
         <v>15</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D150" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
+        <v>269</v>
+      </c>
+      <c r="B151" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B151" s="2" t="s">
-        <v>271</v>
-      </c>
       <c r="C151" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D151" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
+        <v>271</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="C152" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D152" t="s">
         <v>273</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D152" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
+        <v>274</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B153" s="2" t="s">
-        <v>276</v>
-      </c>
       <c r="C153" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D153" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
+        <v>276</v>
+      </c>
+      <c r="B154" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B154" s="2" t="s">
-        <v>278</v>
-      </c>
       <c r="C154" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D154" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B155" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D155" t="s">
         <v>15</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D155" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
+        <v>279</v>
+      </c>
+      <c r="B156" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B156" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="C156" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D156" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
+        <v>281</v>
+      </c>
+      <c r="B157" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B157" s="2" t="s">
-        <v>283</v>
-      </c>
       <c r="C157" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D157" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
+        <v>283</v>
+      </c>
+      <c r="B158" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B158" s="2" t="s">
-        <v>285</v>
-      </c>
       <c r="C158" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D158" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
+        <v>285</v>
+      </c>
+      <c r="B159" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B159" s="2" t="s">
-        <v>287</v>
-      </c>
       <c r="C159" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D159" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>287</v>
+      </c>
+      <c r="B160" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B160" s="2" t="s">
-        <v>289</v>
-      </c>
       <c r="C160" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D160" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D161" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
+        <v>290</v>
+      </c>
+      <c r="B162" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B162" s="2" t="s">
-        <v>292</v>
-      </c>
       <c r="C162" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D162" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
+        <v>292</v>
+      </c>
+      <c r="B163" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B163" s="2" t="s">
-        <v>294</v>
-      </c>
       <c r="C163" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D163" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
+        <v>294</v>
+      </c>
+      <c r="B164" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B164" s="2" t="s">
-        <v>296</v>
-      </c>
       <c r="C164" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D164" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
+        <v>296</v>
+      </c>
+      <c r="B165" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B165" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="C165" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D165" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
+        <v>298</v>
+      </c>
+      <c r="B166" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B166" s="2" t="s">
-        <v>300</v>
-      </c>
       <c r="C166" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D166" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
+        <v>300</v>
+      </c>
+      <c r="B167" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B167" s="2" t="s">
-        <v>302</v>
-      </c>
       <c r="C167" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D167" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
+        <v>302</v>
+      </c>
+      <c r="B168" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B168" s="2" t="s">
-        <v>304</v>
-      </c>
       <c r="C168" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D168" t="s">
         <v>1</v>
@@ -4093,663 +4112,663 @@
     </row>
     <row r="169" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
+        <v>304</v>
+      </c>
+      <c r="B169" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B169" s="2" t="s">
-        <v>306</v>
-      </c>
       <c r="C169" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D169" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
+        <v>306</v>
+      </c>
+      <c r="B170" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B170" s="2" t="s">
-        <v>308</v>
-      </c>
       <c r="C170" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D170" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
+        <v>308</v>
+      </c>
+      <c r="B171" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B171" s="2" t="s">
-        <v>310</v>
-      </c>
       <c r="C171" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D171" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
+        <v>310</v>
+      </c>
+      <c r="B172" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B172" s="2" t="s">
-        <v>312</v>
-      </c>
       <c r="C172" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D172" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
+        <v>312</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B173" s="2" t="s">
-        <v>314</v>
-      </c>
       <c r="C173" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D173" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
+        <v>314</v>
+      </c>
+      <c r="B174" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="B174" s="2" t="s">
-        <v>316</v>
-      </c>
       <c r="C174" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D174" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
+        <v>316</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B175" s="2" t="s">
-        <v>318</v>
-      </c>
       <c r="C175" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D175" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
+        <v>318</v>
+      </c>
+      <c r="B176" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B176" s="2" t="s">
-        <v>320</v>
-      </c>
       <c r="C176" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D176" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
+        <v>320</v>
+      </c>
+      <c r="B177" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B177" s="2" t="s">
-        <v>322</v>
-      </c>
       <c r="C177" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D177" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B178" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D178" t="s">
         <v>15</v>
-      </c>
-      <c r="C178" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D178" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B179" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D179" t="s">
         <v>15</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D179" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
+        <v>324</v>
+      </c>
+      <c r="B180" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B180" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="C180" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D180" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B181" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D181" t="s">
         <v>15</v>
-      </c>
-      <c r="C181" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D181" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
+        <v>327</v>
+      </c>
+      <c r="B182" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B182" s="2" t="s">
-        <v>329</v>
-      </c>
       <c r="C182" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D182" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B183" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D183" t="s">
         <v>15</v>
-      </c>
-      <c r="C183" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D183" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
+        <v>330</v>
+      </c>
+      <c r="B184" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B184" s="2" t="s">
-        <v>332</v>
-      </c>
       <c r="C184" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D184" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
+        <v>332</v>
+      </c>
+      <c r="B185" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B185" s="2" t="s">
-        <v>334</v>
-      </c>
       <c r="C185" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D185" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
+        <v>334</v>
+      </c>
+      <c r="B186" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B186" s="2" t="s">
-        <v>336</v>
-      </c>
       <c r="C186" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D186" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
+        <v>336</v>
+      </c>
+      <c r="B187" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="B187" s="2" t="s">
-        <v>338</v>
-      </c>
       <c r="C187" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D187" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
+        <v>338</v>
+      </c>
+      <c r="B188" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B188" s="2" t="s">
-        <v>340</v>
-      </c>
       <c r="C188" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D188" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B189" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D189" t="s">
         <v>15</v>
-      </c>
-      <c r="C189" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D189" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
+        <v>341</v>
+      </c>
+      <c r="B190" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B190" s="2" t="s">
-        <v>343</v>
-      </c>
       <c r="C190" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D190" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B191" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D191" t="s">
         <v>15</v>
-      </c>
-      <c r="C191" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D191" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
+        <v>344</v>
+      </c>
+      <c r="B192" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B192" s="2" t="s">
-        <v>346</v>
-      </c>
       <c r="C192" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D192" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="193" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
+        <v>346</v>
+      </c>
+      <c r="B193" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="B193" s="2" t="s">
-        <v>348</v>
-      </c>
       <c r="C193" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D193" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="194" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
+        <v>348</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B194" s="2" t="s">
-        <v>350</v>
-      </c>
       <c r="C194" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D194" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="195" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
+        <v>350</v>
+      </c>
+      <c r="B195" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B195" s="2" t="s">
-        <v>352</v>
-      </c>
       <c r="C195" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D195" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="196" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
+        <v>352</v>
+      </c>
+      <c r="B196" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="B196" s="2" t="s">
-        <v>354</v>
-      </c>
       <c r="C196" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D196" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="197" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C197" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="F197" s="3" t="s">
         <v>418</v>
-      </c>
-      <c r="D197" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E197" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="F197" s="3" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
+        <v>355</v>
+      </c>
+      <c r="B198" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="B198" s="2" t="s">
-        <v>357</v>
-      </c>
       <c r="C198" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D198" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="199" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
+        <v>357</v>
+      </c>
+      <c r="B199" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="B199" s="2" t="s">
-        <v>359</v>
-      </c>
       <c r="C199" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D199" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="200" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B200" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D200" t="s">
         <v>15</v>
-      </c>
-      <c r="C200" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D200" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="201" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
+        <v>360</v>
+      </c>
+      <c r="B201" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B201" s="2" t="s">
-        <v>362</v>
-      </c>
       <c r="C201" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D201" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="202" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
+        <v>362</v>
+      </c>
+      <c r="B202" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="B202" s="2" t="s">
-        <v>364</v>
-      </c>
       <c r="C202" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D202" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="203" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B203" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D203" t="s">
         <v>15</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D203" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="204" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
+        <v>365</v>
+      </c>
+      <c r="B204" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B204" s="2" t="s">
-        <v>367</v>
-      </c>
       <c r="C204" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D204" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="205" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
+        <v>367</v>
+      </c>
+      <c r="B205" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="B205" s="2" t="s">
-        <v>369</v>
-      </c>
       <c r="C205" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D205" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="206" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
+        <v>369</v>
+      </c>
+      <c r="B206" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B206" s="2" t="s">
-        <v>371</v>
-      </c>
       <c r="C206" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D206" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="207" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B207" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D207" t="s">
         <v>15</v>
-      </c>
-      <c r="C207" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D207" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="208" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
+        <v>372</v>
+      </c>
+      <c r="B208" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="B208" s="2" t="s">
-        <v>374</v>
-      </c>
       <c r="C208" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D208" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
+        <v>374</v>
+      </c>
+      <c r="B209" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B209" s="2" t="s">
-        <v>376</v>
-      </c>
       <c r="C209" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D209" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
+        <v>376</v>
+      </c>
+      <c r="B210" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="B210" s="2" t="s">
-        <v>378</v>
-      </c>
       <c r="C210" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D210" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
+        <v>378</v>
+      </c>
+      <c r="B211" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="B211" s="2" t="s">
-        <v>380</v>
-      </c>
       <c r="C211" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D211" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
+        <v>380</v>
+      </c>
+      <c r="B212" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B212" s="2" t="s">
-        <v>382</v>
-      </c>
       <c r="C212" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D212" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
+        <v>382</v>
+      </c>
+      <c r="B213" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B213" s="2" t="s">
-        <v>384</v>
-      </c>
       <c r="C213" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D213" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B214" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D214" t="s">
         <v>15</v>
-      </c>
-      <c r="C214" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D214" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
+        <v>385</v>
+      </c>
+      <c r="B215" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B215" s="2" t="s">
-        <v>387</v>
-      </c>
       <c r="C215" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D215" t="s">
         <v>1</v>
@@ -4757,170 +4776,170 @@
     </row>
     <row r="216" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
+        <v>387</v>
+      </c>
+      <c r="B216" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="B216" s="2" t="s">
-        <v>389</v>
-      </c>
       <c r="C216" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D216" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="217" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
+        <v>389</v>
+      </c>
+      <c r="B217" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B217" s="2" t="s">
-        <v>391</v>
-      </c>
       <c r="C217" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D217" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="218" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
+        <v>391</v>
+      </c>
+      <c r="B218" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B218" s="2" t="s">
-        <v>393</v>
-      </c>
       <c r="C218" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D218" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="219" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D219" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="220" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
+        <v>394</v>
+      </c>
+      <c r="B220" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B220" s="2" t="s">
-        <v>396</v>
-      </c>
       <c r="C220" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D220" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
+        <v>396</v>
+      </c>
+      <c r="B221" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B221" s="2" t="s">
-        <v>398</v>
-      </c>
       <c r="C221" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D221" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
+        <v>398</v>
+      </c>
+      <c r="B222" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B222" s="2" t="s">
-        <v>400</v>
-      </c>
       <c r="C222" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D222" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="223" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B223" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D223" t="s">
         <v>15</v>
-      </c>
-      <c r="C223" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D223" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B224" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D224" t="s">
         <v>15</v>
-      </c>
-      <c r="C224" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D224" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
+        <v>402</v>
+      </c>
+      <c r="B225" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="B225" s="2" t="s">
-        <v>404</v>
-      </c>
       <c r="C225" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D225" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="226" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
+        <v>404</v>
+      </c>
+      <c r="B226" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="B226" s="2" t="s">
-        <v>406</v>
-      </c>
       <c r="C226" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D226" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="227" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B227" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D227" t="s">
         <v>15</v>
-      </c>
-      <c r="C227" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="D227" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New sheet in the Master Info with context.
</commit_message>
<xml_diff>
--- a/Master Info.xlsx
+++ b/Master Info.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryansmith/Documents/Coding/topomapper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23D60C6-0B1C-F442-968A-981C31D240DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E1111B-11CF-4644-9DDA-CE449085A65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Info" sheetId="2" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Connection1" localSheetId="0">Sheet1!$A$2:$D$227</definedName>
-    <definedName name="streetInfo" localSheetId="0">Sheet1!$A$2:$D$227</definedName>
+    <definedName name="Connection1" localSheetId="1">Data!$A$2:$D$227</definedName>
+    <definedName name="streetInfo" localSheetId="1">Data!$A$2:$D$227</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="444">
   <si>
     <t>Name</t>
   </si>
@@ -1329,13 +1330,73 @@
   </si>
   <si>
     <t>Named for Albert Joseph Anthony, Chairman of the Townsville Harbour Board in the mid 20&lt;sup&gt;th&lt;/sup&gt; century (Mathew, 2008, p. 9). As a business person, Anthony took over the &lt;i&gt;All Nations Warehouse&lt;/i&gt; import business along with their mother Wadiha (Monsour, 2017), both of who were members of the Lebanese community in North Queensland. More personally, it is clear that Anthony was a prominent figure in the community, with a full page description of his marriage to Mena Sarks suggesting that it was a \"wedding of interest to country folk of N.S.W. and Queensland\" (\"WEDDING BELLS\", 1937, p. 8). In one engagement notice, Anthony is described as "a nephew of his Beautitude Patriarch Arida, of Antioch" ("ENGAGEMENT NOTICES", 1936, p. 1).</t>
+  </si>
+  <si>
+    <t>Updated in app</t>
+  </si>
+  <si>
+    <t>Information Breakdown</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>The thematic code for where the street fits. One of atsi, business, etc, euexpl, local, monarchy, none, pol, religious, transplants or war.</t>
+  </si>
+  <si>
+    <t>Yes if an image of the odonym's namesake is found/had.</t>
+  </si>
+  <si>
+    <t>Yes if the referenced material (primary or secondary sources) have been archived. For copyright reasons, this data is not included in the code repo.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Yes if the description provided in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Description</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> reflects what is in the datafiles/&lt;theme&gt;.json file.</t>
+    </r>
+  </si>
+  <si>
+    <t>Any notes that are needed for future reference.</t>
+  </si>
+  <si>
+    <t>Name of the odonym.</t>
+  </si>
+  <si>
+    <t>HTML formatted description of the namesake of the odonym.</t>
+  </si>
+  <si>
+    <t>HTML formatted APA references.</t>
+  </si>
+  <si>
+    <t>To-Do</t>
+  </si>
+  <si>
+    <t>The primary focus now is on fleshing out the information for each odonym so that the namesake is not the only piece of information. As the app stands, much of the information available is of the "it is named for" type without elaboration or context.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1348,8 +1409,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1374,8 +1449,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1383,12 +1464,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1405,6 +1527,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26" customBuiltin="1"/>
@@ -1723,12 +1862,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7667E48D-EA88-284A-8D01-5DF85B19F789}">
+  <dimension ref="B4:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="84.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="B11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B12" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="C18" s="14"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="13"/>
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="13"/>
+      <c r="C20" s="14"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="760" topLeftCell="A3" activePane="bottomLeft"/>
-      <selection activeCell="B2" sqref="B2"/>
+      <pane ySplit="760" topLeftCell="A105"/>
+      <selection sqref="A1:XFD1"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated Armati Street info with picture.
</commit_message>
<xml_diff>
--- a/Master Info.xlsx
+++ b/Master Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryansmith/Documents/Coding/topomapper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C005D5-7854-E442-A7E3-6DE7E8630AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1887D753-C255-F642-9C27-2B6C8A233964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="451">
   <si>
     <t>Name</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t xml:space="preserve">Armati Street </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Named for Pio Vico Armati (see Mathew, 1979), late 19th and early 20th century. Owned and operated multiple chemist shops on Flinders Street (Mathew, 2008, p. 10). </t>
   </si>
   <si>
     <t xml:space="preserve">Arundel Court </t>
@@ -1405,6 +1402,12 @@
   </si>
   <si>
     <t>Named for Archibald Archer, member of the Legislative Assembly in the late 19&lt;sup&gt;th&lt;/sup&gt; century who \"served in the McIlwraith Ministry as Colonial Treasurer and Secretary for Public Instruction in 1882-83\" (Mathew, 2008, p. 10). Born in Scotland in 1820, he moved to Australia and worked on plantations across the Pacific, specifically Hawaii (in the U.S.A.) and the South Seas (State Library of Queensland, 2022). In an obituary, Archer is described as being a key part of the passage of the Land Act of 1868 (\"OBITUARY: MR. ARCHIBALD ARCHER,\" 1902, p. 5) - the \"father\" of the Land Act as he was referred to by other MPs (Queensland, 1875) - which was described thusly in an op-ed in 1868: \"the land is our capital, and the new Act is intended to liberate it [from Sydneysider financiers], so that we can turn it to our beneficial use\" (\"THE NEW QUEENSLAND LAND ACT\" 1868, p. 3).</t>
+  </si>
+  <si>
+    <t>Mathew, J. (2008). &lt;i&gt;Highways and Byways: The Origin of Townsville Street Names&lt;/i&gt; (Revised ed.). Townsville, QLD: Townsville Library Service.&lt;p&gt;&lt;/p&gt;OBITUARY: MR. P. V. ARMATI. (1923, Dec 6). &lt;i&gt;Daily Mercury&lt;/i&gt;, p. 4.&lt;p&gt;&lt;/p&gt;TELEGRAPHIC INTELLIGENCE. (1887, May 23). &lt;i&gt;The Northern Miner&lt;/i&gt;, p. 3.</t>
+  </si>
+  <si>
+    <t>Named for Pio Vico Armati who owned and operated multiple chemist shops on Flinders Street (Mathew, 2008, p. 10). Originally from Rome, Armati lived in Townsville for more than 50 years after a successful career at a Roman university (\"OBITUARY: MR. P. V. ARMATI\", 1923). In the 1880s, he became a trustee for the Botanical Gardens Reserve in town (\"TELEGRAPHIC INTELLIGENCE\", 1887).</t>
   </si>
 </sst>
 </file>
@@ -1976,22 +1979,22 @@
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="25" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C4" s="26"/>
       <c r="E4" s="12" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -1999,10 +2002,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -2010,10 +2013,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -2021,10 +2024,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="34" x14ac:dyDescent="0.2">
@@ -2032,7 +2035,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -2040,7 +2043,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="34" x14ac:dyDescent="0.2">
@@ -2048,15 +2051,15 @@
         <v>5</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -2064,18 +2067,18 @@
         <v>7</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="25" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C17" s="26"/>
     </row>
     <row r="18" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="27" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C18" s="28"/>
     </row>
@@ -2105,10 +2108,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="760" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="760" topLeftCell="A2" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2205,10 +2208,10 @@
         <v>19</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>16</v>
@@ -2231,10 +2234,10 @@
         <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>23</v>
@@ -2250,15 +2253,15 @@
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>450</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>449</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -2270,16 +2273,16 @@
     </row>
     <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -2288,16 +2291,16 @@
     </row>
     <row r="8" spans="1:8" s="24" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="C8" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="22" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>31</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
@@ -2306,10 +2309,10 @@
     </row>
     <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>22</v>
@@ -2324,16 +2327,16 @@
     </row>
     <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -2342,10 +2345,10 @@
     </row>
     <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>22</v>
@@ -2360,16 +2363,16 @@
     </row>
     <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -2378,16 +2381,16 @@
     </row>
     <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2396,16 +2399,16 @@
     </row>
     <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2414,10 +2417,10 @@
     </row>
     <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>22</v>
@@ -2432,10 +2435,10 @@
     </row>
     <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>22</v>
@@ -2450,16 +2453,16 @@
     </row>
     <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -2468,16 +2471,16 @@
     </row>
     <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -2486,10 +2489,10 @@
     </row>
     <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>22</v>
@@ -2504,16 +2507,16 @@
     </row>
     <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="C20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -2522,10 +2525,10 @@
     </row>
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>22</v>
@@ -2540,10 +2543,10 @@
     </row>
     <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>22</v>
@@ -2558,16 +2561,16 @@
     </row>
     <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -2576,16 +2579,16 @@
     </row>
     <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -2594,16 +2597,16 @@
     </row>
     <row r="25" spans="1:8" s="24" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="22" t="s">
         <v>30</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>31</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
@@ -2612,10 +2615,10 @@
     </row>
     <row r="26" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>22</v>
@@ -2630,16 +2633,16 @@
     </row>
     <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="C27" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -2648,10 +2651,10 @@
     </row>
     <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>22</v>
@@ -2666,16 +2669,16 @@
     </row>
     <row r="29" spans="1:8" s="24" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="22" t="s">
         <v>30</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>31</v>
       </c>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
@@ -2684,16 +2687,16 @@
     </row>
     <row r="30" spans="1:8" s="24" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="22" t="s">
         <v>30</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>31</v>
       </c>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
@@ -2702,16 +2705,16 @@
     </row>
     <row r="31" spans="1:8" s="24" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="23" t="s">
-        <v>78</v>
-      </c>
       <c r="C31" s="23" t="s">
         <v>22</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
@@ -2720,16 +2723,16 @@
     </row>
     <row r="32" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="C32" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2738,16 +2741,16 @@
     </row>
     <row r="33" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2756,10 +2759,10 @@
     </row>
     <row r="34" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>22</v>
@@ -2774,10 +2777,10 @@
     </row>
     <row r="35" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>22</v>
@@ -2792,16 +2795,16 @@
     </row>
     <row r="36" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="C36" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2810,16 +2813,16 @@
     </row>
     <row r="37" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="C37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2828,16 +2831,16 @@
     </row>
     <row r="38" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="C38" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2846,10 +2849,10 @@
     </row>
     <row r="39" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>22</v>
@@ -2864,16 +2867,16 @@
     </row>
     <row r="40" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="C40" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2882,16 +2885,16 @@
     </row>
     <row r="41" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="C41" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2900,16 +2903,16 @@
     </row>
     <row r="42" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="C42" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -2918,10 +2921,10 @@
     </row>
     <row r="43" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>22</v>
@@ -2936,16 +2939,16 @@
     </row>
     <row r="44" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2954,16 +2957,16 @@
     </row>
     <row r="45" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -2972,10 +2975,10 @@
     </row>
     <row r="46" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>22</v>
@@ -2990,10 +2993,10 @@
     </row>
     <row r="47" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>22</v>
@@ -3008,16 +3011,16 @@
     </row>
     <row r="48" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="C48" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -3026,10 +3029,10 @@
     </row>
     <row r="49" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>22</v>
@@ -3044,16 +3047,16 @@
     </row>
     <row r="50" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="C50" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -3062,10 +3065,10 @@
     </row>
     <row r="51" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>22</v>
@@ -3080,16 +3083,16 @@
     </row>
     <row r="52" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="C52" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -3098,16 +3101,16 @@
     </row>
     <row r="53" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="C53" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -3116,16 +3119,16 @@
     </row>
     <row r="54" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="C54" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -3134,16 +3137,16 @@
     </row>
     <row r="55" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -3152,16 +3155,16 @@
     </row>
     <row r="56" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="C56" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -3170,16 +3173,16 @@
     </row>
     <row r="57" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="C57" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -3188,10 +3191,10 @@
     </row>
     <row r="58" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>22</v>
@@ -3206,16 +3209,16 @@
     </row>
     <row r="59" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="C59" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -3224,16 +3227,16 @@
     </row>
     <row r="60" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -3242,16 +3245,16 @@
     </row>
     <row r="61" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="C61" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -3260,16 +3263,16 @@
     </row>
     <row r="62" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -3278,16 +3281,16 @@
     </row>
     <row r="63" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -3296,10 +3299,10 @@
     </row>
     <row r="64" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>22</v>
@@ -3314,16 +3317,16 @@
     </row>
     <row r="65" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="D65" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>12</v>
@@ -3334,16 +3337,16 @@
     </row>
     <row r="66" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -3352,10 +3355,10 @@
     </row>
     <row r="67" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>22</v>
@@ -3370,10 +3373,10 @@
     </row>
     <row r="68" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>22</v>
@@ -3388,16 +3391,16 @@
     </row>
     <row r="69" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="C69" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -3406,16 +3409,16 @@
     </row>
     <row r="70" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -3424,16 +3427,16 @@
     </row>
     <row r="71" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -3442,10 +3445,10 @@
     </row>
     <row r="72" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>22</v>
@@ -3460,16 +3463,16 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="C73" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -3478,16 +3481,16 @@
     </row>
     <row r="74" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -3496,16 +3499,16 @@
     </row>
     <row r="75" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="C75" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -3514,10 +3517,10 @@
     </row>
     <row r="76" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>22</v>
@@ -3532,16 +3535,16 @@
     </row>
     <row r="77" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="C77" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -3550,10 +3553,10 @@
     </row>
     <row r="78" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>22</v>
@@ -3568,16 +3571,16 @@
     </row>
     <row r="79" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="C79" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -3586,10 +3589,10 @@
     </row>
     <row r="80" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>22</v>
@@ -3604,10 +3607,10 @@
     </row>
     <row r="81" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>22</v>
@@ -3622,16 +3625,16 @@
     </row>
     <row r="82" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="C82" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
@@ -3640,16 +3643,16 @@
     </row>
     <row r="83" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>171</v>
-      </c>
       <c r="C83" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
@@ -3658,10 +3661,10 @@
     </row>
     <row r="84" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>22</v>
@@ -3676,16 +3679,16 @@
     </row>
     <row r="85" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="C85" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
@@ -3694,10 +3697,10 @@
     </row>
     <row r="86" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>22</v>
@@ -3712,16 +3715,16 @@
     </row>
     <row r="87" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
@@ -3730,16 +3733,16 @@
     </row>
     <row r="88" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="C88" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -3748,16 +3751,16 @@
     </row>
     <row r="89" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="C89" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
@@ -3766,10 +3769,10 @@
     </row>
     <row r="90" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>22</v>
@@ -3784,16 +3787,16 @@
     </row>
     <row r="91" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>186</v>
-      </c>
       <c r="C91" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
@@ -3802,16 +3805,16 @@
     </row>
     <row r="92" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B92" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
@@ -3820,16 +3823,16 @@
     </row>
     <row r="93" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B93" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="C93" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
@@ -3838,10 +3841,10 @@
     </row>
     <row r="94" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>22</v>
@@ -3856,10 +3859,10 @@
     </row>
     <row r="95" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>22</v>
@@ -3874,16 +3877,16 @@
     </row>
     <row r="96" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="C96" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
@@ -3892,10 +3895,10 @@
     </row>
     <row r="97" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>22</v>
@@ -3910,16 +3913,16 @@
     </row>
     <row r="98" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B98" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
@@ -3928,16 +3931,16 @@
     </row>
     <row r="99" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B99" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -3946,16 +3949,16 @@
     </row>
     <row r="100" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B100" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
@@ -3964,16 +3967,16 @@
     </row>
     <row r="101" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B101" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="C101" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
@@ -3982,10 +3985,10 @@
     </row>
     <row r="102" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>22</v>
@@ -4000,16 +4003,16 @@
     </row>
     <row r="103" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>206</v>
-      </c>
       <c r="C103" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
@@ -4018,16 +4021,16 @@
     </row>
     <row r="104" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B104" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
@@ -4036,16 +4039,16 @@
     </row>
     <row r="105" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B105" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
@@ -4054,16 +4057,16 @@
     </row>
     <row r="106" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B106" s="2" t="s">
-        <v>210</v>
-      </c>
       <c r="C106" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
@@ -4072,16 +4075,16 @@
     </row>
     <row r="107" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B107" s="2" t="s">
-        <v>212</v>
-      </c>
       <c r="C107" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
@@ -4090,16 +4093,16 @@
     </row>
     <row r="108" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B108" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
@@ -4108,16 +4111,16 @@
     </row>
     <row r="109" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B109" s="2" t="s">
-        <v>215</v>
-      </c>
       <c r="C109" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
@@ -4126,10 +4129,10 @@
     </row>
     <row r="110" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>22</v>
@@ -4144,10 +4147,10 @@
     </row>
     <row r="111" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>22</v>
@@ -4162,16 +4165,16 @@
     </row>
     <row r="112" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B112" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
@@ -4180,16 +4183,16 @@
     </row>
     <row r="113" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="C113" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
@@ -4198,16 +4201,16 @@
     </row>
     <row r="114" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B114" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="C114" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
@@ -4216,16 +4219,16 @@
     </row>
     <row r="115" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B115" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
@@ -4234,10 +4237,10 @@
     </row>
     <row r="116" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>22</v>
@@ -4252,10 +4255,10 @@
     </row>
     <row r="117" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>22</v>
@@ -4270,16 +4273,16 @@
     </row>
     <row r="118" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B118" s="2" t="s">
-        <v>229</v>
-      </c>
       <c r="C118" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
@@ -4288,16 +4291,16 @@
     </row>
     <row r="119" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B119" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
@@ -4306,10 +4309,10 @@
     </row>
     <row r="120" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>232</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>22</v>
@@ -4324,10 +4327,10 @@
     </row>
     <row r="121" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>22</v>
@@ -4342,10 +4345,10 @@
     </row>
     <row r="122" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B122" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>22</v>
@@ -4360,16 +4363,16 @@
     </row>
     <row r="123" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B123" s="2" t="s">
-        <v>237</v>
-      </c>
       <c r="C123" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
@@ -4378,16 +4381,16 @@
     </row>
     <row r="124" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B124" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
@@ -4396,16 +4399,16 @@
     </row>
     <row r="125" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B125" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="C125" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D125" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
@@ -4414,10 +4417,10 @@
     </row>
     <row r="126" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B126" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>22</v>
@@ -4432,16 +4435,16 @@
     </row>
     <row r="127" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B127" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D127" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
@@ -4450,10 +4453,10 @@
     </row>
     <row r="128" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>22</v>
@@ -4468,16 +4471,16 @@
     </row>
     <row r="129" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B129" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B129" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="C129" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
@@ -4486,16 +4489,16 @@
     </row>
     <row r="130" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B130" s="2" t="s">
-        <v>249</v>
-      </c>
       <c r="C130" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
@@ -4504,10 +4507,10 @@
     </row>
     <row r="131" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B131" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>22</v>
@@ -4522,16 +4525,16 @@
     </row>
     <row r="132" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B132" s="2" t="s">
-        <v>253</v>
-      </c>
       <c r="C132" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
@@ -4540,16 +4543,16 @@
     </row>
     <row r="133" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B133" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>255</v>
-      </c>
       <c r="C133" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
@@ -4558,10 +4561,10 @@
     </row>
     <row r="134" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B134" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>257</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>22</v>
@@ -4576,16 +4579,16 @@
     </row>
     <row r="135" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B135" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B135" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="C135" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
@@ -4594,16 +4597,16 @@
     </row>
     <row r="136" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B136" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B136" s="2" t="s">
-        <v>261</v>
-      </c>
       <c r="C136" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
@@ -4612,16 +4615,16 @@
     </row>
     <row r="137" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
@@ -4630,16 +4633,16 @@
     </row>
     <row r="138" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B138" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B138" s="2" t="s">
-        <v>264</v>
-      </c>
       <c r="C138" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
@@ -4648,16 +4651,16 @@
     </row>
     <row r="139" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B139" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B139" s="2" t="s">
-        <v>266</v>
-      </c>
       <c r="C139" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
@@ -4666,10 +4669,10 @@
     </row>
     <row r="140" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B140" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>268</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>22</v>
@@ -4684,10 +4687,10 @@
     </row>
     <row r="141" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>22</v>
@@ -4702,10 +4705,10 @@
     </row>
     <row r="142" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>22</v>
@@ -4720,10 +4723,10 @@
     </row>
     <row r="143" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>273</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>22</v>
@@ -4738,16 +4741,16 @@
     </row>
     <row r="144" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B144" s="2" t="s">
-        <v>275</v>
-      </c>
       <c r="C144" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
@@ -4756,10 +4759,10 @@
     </row>
     <row r="145" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>277</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>22</v>
@@ -4774,10 +4777,10 @@
     </row>
     <row r="146" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>279</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>22</v>
@@ -4792,16 +4795,16 @@
     </row>
     <row r="147" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B147" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="C147" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
@@ -4810,10 +4813,10 @@
     </row>
     <row r="148" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>22</v>
@@ -4828,16 +4831,16 @@
     </row>
     <row r="149" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B149" s="2" t="s">
-        <v>285</v>
-      </c>
       <c r="C149" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
@@ -4846,16 +4849,16 @@
     </row>
     <row r="150" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B150" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D150" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
@@ -4864,10 +4867,10 @@
     </row>
     <row r="151" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B151" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>288</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>22</v>
@@ -4882,16 +4885,16 @@
     </row>
     <row r="152" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="C152" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D152" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="E152" s="1"/>
       <c r="F152" s="1"/>
@@ -4900,16 +4903,16 @@
     </row>
     <row r="153" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B153" s="2" t="s">
-        <v>293</v>
-      </c>
       <c r="C153" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E153" s="1"/>
       <c r="F153" s="1"/>
@@ -4918,10 +4921,10 @@
     </row>
     <row r="154" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B154" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>22</v>
@@ -4936,16 +4939,16 @@
     </row>
     <row r="155" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B155" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D155" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E155" s="1"/>
       <c r="F155" s="1"/>
@@ -4954,16 +4957,16 @@
     </row>
     <row r="156" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B156" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B156" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="C156" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E156" s="1"/>
       <c r="F156" s="1"/>
@@ -4972,10 +4975,10 @@
     </row>
     <row r="157" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B157" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>22</v>
@@ -4990,10 +4993,10 @@
     </row>
     <row r="158" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B158" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>302</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>22</v>
@@ -5008,16 +5011,16 @@
     </row>
     <row r="159" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B159" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B159" s="2" t="s">
-        <v>304</v>
-      </c>
       <c r="C159" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E159" s="1"/>
       <c r="F159" s="1"/>
@@ -5026,10 +5029,10 @@
     </row>
     <row r="160" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B160" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>306</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>22</v>
@@ -5044,10 +5047,10 @@
     </row>
     <row r="161" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>22</v>
@@ -5062,16 +5065,16 @@
     </row>
     <row r="162" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B162" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B162" s="2" t="s">
-        <v>309</v>
-      </c>
       <c r="C162" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E162" s="1"/>
       <c r="F162" s="1"/>
@@ -5080,16 +5083,16 @@
     </row>
     <row r="163" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B163" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B163" s="2" t="s">
-        <v>311</v>
-      </c>
       <c r="C163" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E163" s="1"/>
       <c r="F163" s="1"/>
@@ -5098,16 +5101,16 @@
     </row>
     <row r="164" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B164" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="B164" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="C164" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E164" s="1"/>
       <c r="F164" s="1"/>
@@ -5116,16 +5119,16 @@
     </row>
     <row r="165" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B165" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B165" s="2" t="s">
-        <v>315</v>
-      </c>
       <c r="C165" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E165" s="1"/>
       <c r="F165" s="1"/>
@@ -5134,16 +5137,16 @@
     </row>
     <row r="166" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B166" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="B166" s="2" t="s">
-        <v>317</v>
-      </c>
       <c r="C166" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E166" s="1"/>
       <c r="F166" s="1"/>
@@ -5152,16 +5155,16 @@
     </row>
     <row r="167" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B167" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="B167" s="2" t="s">
-        <v>319</v>
-      </c>
       <c r="C167" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E167" s="1"/>
       <c r="F167" s="1"/>
@@ -5170,10 +5173,10 @@
     </row>
     <row r="168" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B168" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>22</v>
@@ -5188,10 +5191,10 @@
     </row>
     <row r="169" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B169" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>323</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>22</v>
@@ -5206,16 +5209,16 @@
     </row>
     <row r="170" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B170" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B170" s="2" t="s">
-        <v>325</v>
-      </c>
       <c r="C170" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E170" s="1"/>
       <c r="F170" s="1"/>
@@ -5224,10 +5227,10 @@
     </row>
     <row r="171" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B171" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>327</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>22</v>
@@ -5242,10 +5245,10 @@
     </row>
     <row r="172" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B172" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>329</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>22</v>
@@ -5260,16 +5263,16 @@
     </row>
     <row r="173" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B173" s="2" t="s">
-        <v>331</v>
-      </c>
       <c r="C173" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E173" s="1"/>
       <c r="F173" s="1"/>
@@ -5278,16 +5281,16 @@
     </row>
     <row r="174" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B174" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B174" s="2" t="s">
-        <v>333</v>
-      </c>
       <c r="C174" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E174" s="1"/>
       <c r="F174" s="1"/>
@@ -5296,10 +5299,10 @@
     </row>
     <row r="175" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>22</v>
@@ -5314,16 +5317,16 @@
     </row>
     <row r="176" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B176" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B176" s="2" t="s">
-        <v>337</v>
-      </c>
       <c r="C176" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E176" s="1"/>
       <c r="F176" s="1"/>
@@ -5332,16 +5335,16 @@
     </row>
     <row r="177" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B177" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B177" s="2" t="s">
-        <v>339</v>
-      </c>
       <c r="C177" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E177" s="1"/>
       <c r="F177" s="1"/>
@@ -5350,16 +5353,16 @@
     </row>
     <row r="178" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B178" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D178" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C178" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E178" s="1"/>
       <c r="F178" s="1"/>
@@ -5368,16 +5371,16 @@
     </row>
     <row r="179" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B179" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D179" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D179" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E179" s="1"/>
       <c r="F179" s="1"/>
@@ -5386,16 +5389,16 @@
     </row>
     <row r="180" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B180" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B180" s="2" t="s">
-        <v>343</v>
-      </c>
       <c r="C180" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E180" s="1"/>
       <c r="F180" s="1"/>
@@ -5404,16 +5407,16 @@
     </row>
     <row r="181" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B181" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D181" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C181" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D181" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E181" s="1"/>
       <c r="F181" s="1"/>
@@ -5422,10 +5425,10 @@
     </row>
     <row r="182" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B182" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>346</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>22</v>
@@ -5440,16 +5443,16 @@
     </row>
     <row r="183" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B183" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D183" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C183" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E183" s="1"/>
       <c r="F183" s="1"/>
@@ -5458,10 +5461,10 @@
     </row>
     <row r="184" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B184" s="2" t="s">
         <v>348</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>349</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>22</v>
@@ -5476,16 +5479,16 @@
     </row>
     <row r="185" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B185" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="B185" s="2" t="s">
-        <v>351</v>
-      </c>
       <c r="C185" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E185" s="1"/>
       <c r="F185" s="1"/>
@@ -5494,10 +5497,10 @@
     </row>
     <row r="186" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B186" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>353</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>22</v>
@@ -5512,16 +5515,16 @@
     </row>
     <row r="187" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B187" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B187" s="2" t="s">
-        <v>355</v>
-      </c>
       <c r="C187" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E187" s="1"/>
       <c r="F187" s="1"/>
@@ -5530,10 +5533,10 @@
     </row>
     <row r="188" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B188" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>357</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>22</v>
@@ -5548,16 +5551,16 @@
     </row>
     <row r="189" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B189" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D189" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C189" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D189" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E189" s="1"/>
       <c r="F189" s="1"/>
@@ -5566,16 +5569,16 @@
     </row>
     <row r="190" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B190" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="B190" s="2" t="s">
-        <v>360</v>
-      </c>
       <c r="C190" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E190" s="1"/>
       <c r="F190" s="1"/>
@@ -5584,16 +5587,16 @@
     </row>
     <row r="191" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B191" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D191" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C191" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E191" s="1"/>
       <c r="F191" s="1"/>
@@ -5602,16 +5605,16 @@
     </row>
     <row r="192" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B192" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B192" s="2" t="s">
-        <v>363</v>
-      </c>
       <c r="C192" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E192" s="1"/>
       <c r="F192" s="1"/>
@@ -5620,16 +5623,16 @@
     </row>
     <row r="193" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B193" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B193" s="2" t="s">
-        <v>365</v>
-      </c>
       <c r="C193" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E193" s="1"/>
       <c r="F193" s="1"/>
@@ -5638,16 +5641,16 @@
     </row>
     <row r="194" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B194" s="2" t="s">
-        <v>367</v>
-      </c>
       <c r="C194" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E194" s="1"/>
       <c r="F194" s="1"/>
@@ -5656,16 +5659,16 @@
     </row>
     <row r="195" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B195" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="B195" s="2" t="s">
-        <v>369</v>
-      </c>
       <c r="C195" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E195" s="1"/>
       <c r="F195" s="1"/>
@@ -5674,16 +5677,16 @@
     </row>
     <row r="196" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B196" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B196" s="2" t="s">
-        <v>371</v>
-      </c>
       <c r="C196" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E196" s="1"/>
       <c r="F196" s="1"/>
@@ -5692,36 +5695,36 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
+        <v>371</v>
+      </c>
+      <c r="B197" t="s">
         <v>372</v>
       </c>
-      <c r="B197" t="s">
+      <c r="C197" t="s">
         <v>373</v>
       </c>
-      <c r="C197" t="s">
-        <v>374</v>
-      </c>
       <c r="D197" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E197" t="s">
         <v>12</v>
       </c>
       <c r="G197" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="198" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B198" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B198" s="2" t="s">
-        <v>377</v>
-      </c>
       <c r="C198" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E198" s="1"/>
       <c r="F198" s="1"/>
@@ -5730,10 +5733,10 @@
     </row>
     <row r="199" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B199" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>379</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>22</v>
@@ -5748,16 +5751,16 @@
     </row>
     <row r="200" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B200" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D200" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C200" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D200" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E200" s="1"/>
       <c r="F200" s="1"/>
@@ -5766,16 +5769,16 @@
     </row>
     <row r="201" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B201" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B201" s="2" t="s">
-        <v>382</v>
-      </c>
       <c r="C201" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E201" s="1"/>
       <c r="F201" s="1"/>
@@ -5784,16 +5787,16 @@
     </row>
     <row r="202" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B202" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B202" s="2" t="s">
-        <v>384</v>
-      </c>
       <c r="C202" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E202" s="1"/>
       <c r="F202" s="1"/>
@@ -5802,16 +5805,16 @@
     </row>
     <row r="203" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B203" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D203" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D203" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E203" s="1"/>
       <c r="F203" s="1"/>
@@ -5820,16 +5823,16 @@
     </row>
     <row r="204" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B204" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B204" s="2" t="s">
-        <v>387</v>
-      </c>
       <c r="C204" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E204" s="1"/>
       <c r="F204" s="1"/>
@@ -5838,10 +5841,10 @@
     </row>
     <row r="205" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B205" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>389</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>22</v>
@@ -5856,10 +5859,10 @@
     </row>
     <row r="206" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B206" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="B206" s="2" t="s">
-        <v>391</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>22</v>
@@ -5874,16 +5877,16 @@
     </row>
     <row r="207" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B207" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D207" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C207" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D207" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E207" s="1"/>
       <c r="F207" s="1"/>
@@ -5892,16 +5895,16 @@
     </row>
     <row r="208" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B208" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B208" s="2" t="s">
-        <v>394</v>
-      </c>
       <c r="C208" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E208" s="1"/>
       <c r="F208" s="1"/>
@@ -5910,16 +5913,16 @@
     </row>
     <row r="209" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B209" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B209" s="2" t="s">
-        <v>396</v>
-      </c>
       <c r="C209" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E209" s="1"/>
       <c r="F209" s="1"/>
@@ -5928,10 +5931,10 @@
     </row>
     <row r="210" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B210" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="B210" s="2" t="s">
-        <v>398</v>
       </c>
       <c r="C210" s="2" t="s">
         <v>22</v>
@@ -5946,16 +5949,16 @@
     </row>
     <row r="211" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B211" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B211" s="2" t="s">
-        <v>400</v>
-      </c>
       <c r="C211" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E211" s="1"/>
       <c r="F211" s="1"/>
@@ -5964,10 +5967,10 @@
     </row>
     <row r="212" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B212" s="2" t="s">
         <v>401</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>402</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>22</v>
@@ -5982,16 +5985,16 @@
     </row>
     <row r="213" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B213" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="B213" s="2" t="s">
-        <v>404</v>
-      </c>
       <c r="C213" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E213" s="1"/>
       <c r="F213" s="1"/>
@@ -6000,16 +6003,16 @@
     </row>
     <row r="214" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B214" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D214" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C214" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D214" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E214" s="1"/>
       <c r="F214" s="1"/>
@@ -6018,10 +6021,10 @@
     </row>
     <row r="215" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B215" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>407</v>
       </c>
       <c r="C215" s="2" t="s">
         <v>22</v>
@@ -6036,16 +6039,16 @@
     </row>
     <row r="216" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B216" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B216" s="2" t="s">
-        <v>409</v>
-      </c>
       <c r="C216" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E216" s="1"/>
       <c r="F216" s="1"/>
@@ -6054,16 +6057,16 @@
     </row>
     <row r="217" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B217" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B217" s="2" t="s">
-        <v>411</v>
-      </c>
       <c r="C217" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E217" s="1"/>
       <c r="F217" s="1"/>
@@ -6072,16 +6075,16 @@
     </row>
     <row r="218" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B218" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="B218" s="2" t="s">
-        <v>413</v>
-      </c>
       <c r="C218" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E218" s="1"/>
       <c r="F218" s="1"/>
@@ -6090,16 +6093,16 @@
     </row>
     <row r="219" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E219" s="1"/>
       <c r="F219" s="1"/>
@@ -6108,10 +6111,10 @@
     </row>
     <row r="220" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B220" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="B220" s="2" t="s">
-        <v>416</v>
       </c>
       <c r="C220" s="2" t="s">
         <v>22</v>
@@ -6126,16 +6129,16 @@
     </row>
     <row r="221" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B221" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="B221" s="2" t="s">
-        <v>418</v>
-      </c>
       <c r="C221" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E221" s="1"/>
       <c r="F221" s="1"/>
@@ -6144,16 +6147,16 @@
     </row>
     <row r="222" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B222" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="B222" s="2" t="s">
-        <v>420</v>
-      </c>
       <c r="C222" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E222" s="1"/>
       <c r="F222" s="1"/>
@@ -6162,16 +6165,16 @@
     </row>
     <row r="223" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B223" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D223" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C223" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D223" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E223" s="1"/>
       <c r="F223" s="1"/>
@@ -6180,16 +6183,16 @@
     </row>
     <row r="224" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B224" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D224" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C224" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D224" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E224" s="1"/>
       <c r="F224" s="1"/>
@@ -6198,10 +6201,10 @@
     </row>
     <row r="225" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B225" s="2" t="s">
         <v>423</v>
-      </c>
-      <c r="B225" s="2" t="s">
-        <v>424</v>
       </c>
       <c r="C225" s="2" t="s">
         <v>22</v>
@@ -6216,16 +6219,16 @@
     </row>
     <row r="226" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B226" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="B226" s="2" t="s">
-        <v>426</v>
-      </c>
       <c r="C226" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E226" s="1"/>
       <c r="F226" s="1"/>
@@ -6234,16 +6237,16 @@
     </row>
     <row r="227" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B227" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D227" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C227" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D227" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E227" s="1"/>
       <c r="F227" s="1"/>

</xml_diff>

<commit_message>
Tweak to Master Info
</commit_message>
<xml_diff>
--- a/Master Info.xlsx
+++ b/Master Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryansmith/Documents/Coding/topomapper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3A02C0-74F7-4546-A063-7FB870DE52E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75015B8-A656-E149-9F23-2C256E96A401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,9 +129,6 @@
     <t xml:space="preserve">Balmoral Drive </t>
   </si>
   <si>
-    <t xml:space="preserve"> Named for "the royal residence in Aberdeenshire," purchased by Prince Albert (Mathew, 2008, p. 13). </t>
-  </si>
-  <si>
     <t xml:space="preserve">Barboutis Street </t>
   </si>
   <si>
@@ -1413,7 +1410,10 @@
     <t>Foyle, J. (2002). A Reconstruction of Thomas Wolsey's Great Hall at Hampton Court Palace. &lt;i&gt;Architectural History, 45&lt;/i&gt;(2), 128-158.&lt;p&gt;&lt;/p&gt;Mathew, J. (2008). &lt;i&gt;Highways and Byways: The Origin of Townsville Street Names&lt;/i&gt; (Revised ed.). Townsville, QLD: Townsville Library Service.&lt;p&gt;&lt;/p&gt;Wiseman, R., Watt, C., Greening, E., Stevens, P. &amp; O'Kefffe, C. (2002). An investigation into the alleged haunting of Hampton Court Palace: Psychological variables and magnetic fields. &lt;i&gt;Journal of Parapsychology, 66&lt;/i&gt;(4), 387-408.</t>
   </si>
   <si>
-    <t>"Named after a palace at Hampton, near London, built by Cardinal Wolsey and enlarged by Henry VIII" (Mathew, 2008, p. 11). When Henry VIII took possession, he undertook a remodelling that lasted ten years, one of many renovation and change projects that has resulted in its original desing being lost to history (Foyle, 2002). An object of curiosity for many who believe in the paranormal, the Palace has been the subject of psychological research that looks to understand how the \"haunting\" of the palace is experienced (see Wiseman et al., 2002). The palace is now a tourist site.</t>
+    <t>\"Named after a palace at Hampton, near London, built by Cardinal Wolsey and enlarged by Henry VIII\" (Mathew, 2008, p. 11). When Henry VIII took possession, he undertook a remodelling that lasted ten years, one of many renovation and change projects that has resulted in its original desing being lost to history (Foyle, 2002). An object of curiosity for many who believe in the paranormal, the Palace has been the subject of psychological research that looks to understand how the \"haunting\" of the palace is experienced (see Wiseman et al., 2002). The palace is now a tourist site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Named for "the royal residence in Aberdeenshire," purchased by Prince Albert (Mathew, 2008, p. 13). </t>
   </si>
 </sst>
 </file>
@@ -1985,22 +1985,22 @@
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="25" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C4" s="26"/>
       <c r="E4" s="12" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -2008,10 +2008,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -2019,10 +2019,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -2030,10 +2030,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="34" x14ac:dyDescent="0.2">
@@ -2041,7 +2041,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -2049,7 +2049,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="34" x14ac:dyDescent="0.2">
@@ -2057,15 +2057,15 @@
         <v>5</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="17" x14ac:dyDescent="0.2">
@@ -2073,18 +2073,18 @@
         <v>7</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="25" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C17" s="26"/>
     </row>
     <row r="18" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="27" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C18" s="28"/>
     </row>
@@ -2117,7 +2117,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="760" topLeftCell="A4" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2214,10 +2214,10 @@
         <v>19</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>16</v>
@@ -2240,10 +2240,10 @@
         <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>23</v>
@@ -2264,10 +2264,10 @@
         <v>24</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>16</v>
@@ -2282,7 +2282,7 @@
         <v>17</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="5" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -2290,10 +2290,10 @@
         <v>25</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>26</v>
@@ -2332,7 +2332,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>452</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>22</v>
@@ -2347,16 +2347,16 @@
     </row>
     <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -2365,10 +2365,10 @@
     </row>
     <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>22</v>
@@ -2383,16 +2383,16 @@
     </row>
     <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -2401,16 +2401,16 @@
     </row>
     <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2419,16 +2419,16 @@
     </row>
     <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2437,10 +2437,10 @@
     </row>
     <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>22</v>
@@ -2455,10 +2455,10 @@
     </row>
     <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>22</v>
@@ -2473,16 +2473,16 @@
     </row>
     <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -2491,16 +2491,16 @@
     </row>
     <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -2509,10 +2509,10 @@
     </row>
     <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>22</v>
@@ -2527,10 +2527,10 @@
     </row>
     <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>22</v>
@@ -2545,10 +2545,10 @@
     </row>
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>22</v>
@@ -2563,10 +2563,10 @@
     </row>
     <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>22</v>
@@ -2581,16 +2581,16 @@
     </row>
     <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -2599,16 +2599,16 @@
     </row>
     <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -2617,7 +2617,7 @@
     </row>
     <row r="25" spans="1:8" s="24" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="23" t="s">
         <v>28</v>
@@ -2635,10 +2635,10 @@
     </row>
     <row r="26" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>22</v>
@@ -2653,10 +2653,10 @@
     </row>
     <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>22</v>
@@ -2671,10 +2671,10 @@
     </row>
     <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>22</v>
@@ -2689,7 +2689,7 @@
     </row>
     <row r="29" spans="1:8" s="24" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B29" s="23" t="s">
         <v>28</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="30" spans="1:8" s="24" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B30" s="23" t="s">
         <v>28</v>
@@ -2725,10 +2725,10 @@
     </row>
     <row r="31" spans="1:8" s="24" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="23" t="s">
         <v>75</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>76</v>
       </c>
       <c r="C31" s="23" t="s">
         <v>22</v>
@@ -2743,10 +2743,10 @@
     </row>
     <row r="32" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>22</v>
@@ -2761,10 +2761,10 @@
     </row>
     <row r="33" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>22</v>
@@ -2779,10 +2779,10 @@
     </row>
     <row r="34" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>22</v>
@@ -2797,10 +2797,10 @@
     </row>
     <row r="35" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>22</v>
@@ -2815,16 +2815,16 @@
     </row>
     <row r="36" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="C36" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2833,16 +2833,16 @@
     </row>
     <row r="37" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="C37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2851,16 +2851,16 @@
     </row>
     <row r="38" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="C38" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2869,10 +2869,10 @@
     </row>
     <row r="39" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>22</v>
@@ -2887,16 +2887,16 @@
     </row>
     <row r="40" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="C40" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2905,16 +2905,16 @@
     </row>
     <row r="41" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="C41" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2923,10 +2923,10 @@
     </row>
     <row r="42" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>22</v>
@@ -2941,10 +2941,10 @@
     </row>
     <row r="43" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>22</v>
@@ -2959,7 +2959,7 @@
     </row>
     <row r="44" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>28</v>
@@ -2977,7 +2977,7 @@
     </row>
     <row r="45" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>28</v>
@@ -2995,10 +2995,10 @@
     </row>
     <row r="46" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>22</v>
@@ -3013,10 +3013,10 @@
     </row>
     <row r="47" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>22</v>
@@ -3031,16 +3031,16 @@
     </row>
     <row r="48" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="C48" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -3049,10 +3049,10 @@
     </row>
     <row r="49" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>22</v>
@@ -3067,10 +3067,10 @@
     </row>
     <row r="50" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>22</v>
@@ -3085,10 +3085,10 @@
     </row>
     <row r="51" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>22</v>
@@ -3103,16 +3103,16 @@
     </row>
     <row r="52" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="C52" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -3121,10 +3121,10 @@
     </row>
     <row r="53" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>22</v>
@@ -3139,16 +3139,16 @@
     </row>
     <row r="54" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="C54" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -3157,7 +3157,7 @@
     </row>
     <row r="55" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>28</v>
@@ -3175,16 +3175,16 @@
     </row>
     <row r="56" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="C56" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -3193,16 +3193,16 @@
     </row>
     <row r="57" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="C57" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -3211,10 +3211,10 @@
     </row>
     <row r="58" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>22</v>
@@ -3229,16 +3229,16 @@
     </row>
     <row r="59" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="C59" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -3247,7 +3247,7 @@
     </row>
     <row r="60" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>28</v>
@@ -3265,16 +3265,16 @@
     </row>
     <row r="61" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="C61" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -3283,7 +3283,7 @@
     </row>
     <row r="62" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>28</v>
@@ -3301,7 +3301,7 @@
     </row>
     <row r="63" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>28</v>
@@ -3319,10 +3319,10 @@
     </row>
     <row r="64" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>22</v>
@@ -3337,16 +3337,16 @@
     </row>
     <row r="65" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="D65" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>12</v>
@@ -3357,7 +3357,7 @@
     </row>
     <row r="66" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>28</v>
@@ -3375,10 +3375,10 @@
     </row>
     <row r="67" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>22</v>
@@ -3393,10 +3393,10 @@
     </row>
     <row r="68" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>22</v>
@@ -3411,16 +3411,16 @@
     </row>
     <row r="69" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="C69" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -3429,7 +3429,7 @@
     </row>
     <row r="70" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>28</v>
@@ -3447,7 +3447,7 @@
     </row>
     <row r="71" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>28</v>
@@ -3465,10 +3465,10 @@
     </row>
     <row r="72" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>22</v>
@@ -3483,16 +3483,16 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="C73" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -3501,7 +3501,7 @@
     </row>
     <row r="74" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>28</v>
@@ -3519,16 +3519,16 @@
     </row>
     <row r="75" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="C75" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -3537,10 +3537,10 @@
     </row>
     <row r="76" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>22</v>
@@ -3555,16 +3555,16 @@
     </row>
     <row r="77" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="C77" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -3573,10 +3573,10 @@
     </row>
     <row r="78" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>22</v>
@@ -3591,10 +3591,10 @@
     </row>
     <row r="79" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>22</v>
@@ -3609,10 +3609,10 @@
     </row>
     <row r="80" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>22</v>
@@ -3627,10 +3627,10 @@
     </row>
     <row r="81" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>22</v>
@@ -3645,16 +3645,16 @@
     </row>
     <row r="82" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="C82" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
@@ -3663,16 +3663,16 @@
     </row>
     <row r="83" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="C83" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
@@ -3681,10 +3681,10 @@
     </row>
     <row r="84" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>22</v>
@@ -3699,16 +3699,16 @@
     </row>
     <row r="85" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>173</v>
-      </c>
       <c r="C85" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
@@ -3717,10 +3717,10 @@
     </row>
     <row r="86" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>22</v>
@@ -3735,7 +3735,7 @@
     </row>
     <row r="87" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>28</v>
@@ -3753,16 +3753,16 @@
     </row>
     <row r="88" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>178</v>
-      </c>
       <c r="C88" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -3771,16 +3771,16 @@
     </row>
     <row r="89" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="C89" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
@@ -3789,10 +3789,10 @@
     </row>
     <row r="90" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>22</v>
@@ -3807,10 +3807,10 @@
     </row>
     <row r="91" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>22</v>
@@ -3825,7 +3825,7 @@
     </row>
     <row r="92" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>28</v>
@@ -3843,16 +3843,16 @@
     </row>
     <row r="93" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B93" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="C93" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
@@ -3861,10 +3861,10 @@
     </row>
     <row r="94" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>22</v>
@@ -3879,10 +3879,10 @@
     </row>
     <row r="95" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>22</v>
@@ -3897,16 +3897,16 @@
     </row>
     <row r="96" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="C96" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
@@ -3915,10 +3915,10 @@
     </row>
     <row r="97" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>22</v>
@@ -3933,7 +3933,7 @@
     </row>
     <row r="98" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>28</v>
@@ -3951,7 +3951,7 @@
     </row>
     <row r="99" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>28</v>
@@ -3969,7 +3969,7 @@
     </row>
     <row r="100" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>28</v>
@@ -3987,16 +3987,16 @@
     </row>
     <row r="101" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B101" s="2" t="s">
-        <v>200</v>
-      </c>
       <c r="C101" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
@@ -4005,10 +4005,10 @@
     </row>
     <row r="102" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>22</v>
@@ -4023,16 +4023,16 @@
     </row>
     <row r="103" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="C103" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
@@ -4041,7 +4041,7 @@
     </row>
     <row r="104" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>28</v>
@@ -4059,7 +4059,7 @@
     </row>
     <row r="105" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>28</v>
@@ -4077,16 +4077,16 @@
     </row>
     <row r="106" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B106" s="2" t="s">
-        <v>208</v>
-      </c>
       <c r="C106" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
@@ -4095,10 +4095,10 @@
     </row>
     <row r="107" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>22</v>
@@ -4113,7 +4113,7 @@
     </row>
     <row r="108" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>28</v>
@@ -4131,16 +4131,16 @@
     </row>
     <row r="109" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B109" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="C109" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
@@ -4149,10 +4149,10 @@
     </row>
     <row r="110" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>22</v>
@@ -4167,10 +4167,10 @@
     </row>
     <row r="111" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>22</v>
@@ -4185,7 +4185,7 @@
     </row>
     <row r="112" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>28</v>
@@ -4203,16 +4203,16 @@
     </row>
     <row r="113" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="C113" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
@@ -4221,16 +4221,16 @@
     </row>
     <row r="114" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B114" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="C114" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
@@ -4239,7 +4239,7 @@
     </row>
     <row r="115" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>28</v>
@@ -4257,10 +4257,10 @@
     </row>
     <row r="116" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>224</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>22</v>
@@ -4275,10 +4275,10 @@
     </row>
     <row r="117" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>22</v>
@@ -4293,16 +4293,16 @@
     </row>
     <row r="118" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B118" s="2" t="s">
-        <v>227</v>
-      </c>
       <c r="C118" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
@@ -4311,7 +4311,7 @@
     </row>
     <row r="119" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>28</v>
@@ -4329,10 +4329,10 @@
     </row>
     <row r="120" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>22</v>
@@ -4347,10 +4347,10 @@
     </row>
     <row r="121" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>22</v>
@@ -4365,10 +4365,10 @@
     </row>
     <row r="122" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B122" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>233</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>22</v>
@@ -4383,16 +4383,16 @@
     </row>
     <row r="123" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B123" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="C123" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
@@ -4401,7 +4401,7 @@
     </row>
     <row r="124" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>28</v>
@@ -4419,16 +4419,16 @@
     </row>
     <row r="125" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B125" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="C125" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D125" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
@@ -4437,10 +4437,10 @@
     </row>
     <row r="126" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B126" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>241</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>22</v>
@@ -4455,7 +4455,7 @@
     </row>
     <row r="127" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>28</v>
@@ -4473,10 +4473,10 @@
     </row>
     <row r="128" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>22</v>
@@ -4491,16 +4491,16 @@
     </row>
     <row r="129" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B129" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B129" s="2" t="s">
-        <v>245</v>
-      </c>
       <c r="C129" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
@@ -4509,10 +4509,10 @@
     </row>
     <row r="130" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>247</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>22</v>
@@ -4527,10 +4527,10 @@
     </row>
     <row r="131" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B131" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>249</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>22</v>
@@ -4545,16 +4545,16 @@
     </row>
     <row r="132" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B132" s="2" t="s">
-        <v>251</v>
-      </c>
       <c r="C132" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
@@ -4563,16 +4563,16 @@
     </row>
     <row r="133" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B133" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>253</v>
-      </c>
       <c r="C133" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
@@ -4581,10 +4581,10 @@
     </row>
     <row r="134" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B134" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>255</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>22</v>
@@ -4599,16 +4599,16 @@
     </row>
     <row r="135" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B135" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B135" s="2" t="s">
-        <v>257</v>
-      </c>
       <c r="C135" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
@@ -4617,16 +4617,16 @@
     </row>
     <row r="136" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B136" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B136" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="C136" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
@@ -4635,16 +4635,16 @@
     </row>
     <row r="137" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
@@ -4653,10 +4653,10 @@
     </row>
     <row r="138" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B138" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>22</v>
@@ -4671,16 +4671,16 @@
     </row>
     <row r="139" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B139" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B139" s="2" t="s">
-        <v>264</v>
-      </c>
       <c r="C139" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
@@ -4689,10 +4689,10 @@
     </row>
     <row r="140" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B140" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>266</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>22</v>
@@ -4707,10 +4707,10 @@
     </row>
     <row r="141" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>22</v>
@@ -4725,10 +4725,10 @@
     </row>
     <row r="142" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>22</v>
@@ -4743,10 +4743,10 @@
     </row>
     <row r="143" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>22</v>
@@ -4761,16 +4761,16 @@
     </row>
     <row r="144" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B144" s="2" t="s">
-        <v>273</v>
-      </c>
       <c r="C144" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
@@ -4779,10 +4779,10 @@
     </row>
     <row r="145" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>275</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>22</v>
@@ -4797,10 +4797,10 @@
     </row>
     <row r="146" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>277</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>22</v>
@@ -4815,16 +4815,16 @@
     </row>
     <row r="147" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B147" s="2" t="s">
-        <v>279</v>
-      </c>
       <c r="C147" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
@@ -4833,10 +4833,10 @@
     </row>
     <row r="148" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>281</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>22</v>
@@ -4851,16 +4851,16 @@
     </row>
     <row r="149" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B149" s="2" t="s">
-        <v>283</v>
-      </c>
       <c r="C149" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
@@ -4869,7 +4869,7 @@
     </row>
     <row r="150" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>28</v>
@@ -4887,10 +4887,10 @@
     </row>
     <row r="151" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B151" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>22</v>
@@ -4905,16 +4905,16 @@
     </row>
     <row r="152" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="C152" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D152" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="E152" s="1"/>
       <c r="F152" s="1"/>
@@ -4923,16 +4923,16 @@
     </row>
     <row r="153" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B153" s="2" t="s">
-        <v>291</v>
-      </c>
       <c r="C153" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E153" s="1"/>
       <c r="F153" s="1"/>
@@ -4941,10 +4941,10 @@
     </row>
     <row r="154" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B154" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>293</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>22</v>
@@ -4959,7 +4959,7 @@
     </row>
     <row r="155" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>28</v>
@@ -4977,16 +4977,16 @@
     </row>
     <row r="156" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B156" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B156" s="2" t="s">
-        <v>296</v>
-      </c>
       <c r="C156" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E156" s="1"/>
       <c r="F156" s="1"/>
@@ -4995,10 +4995,10 @@
     </row>
     <row r="157" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B157" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>298</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>22</v>
@@ -5013,10 +5013,10 @@
     </row>
     <row r="158" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B158" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>22</v>
@@ -5031,16 +5031,16 @@
     </row>
     <row r="159" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B159" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B159" s="2" t="s">
-        <v>302</v>
-      </c>
       <c r="C159" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E159" s="1"/>
       <c r="F159" s="1"/>
@@ -5049,10 +5049,10 @@
     </row>
     <row r="160" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B160" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>304</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>22</v>
@@ -5067,10 +5067,10 @@
     </row>
     <row r="161" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>22</v>
@@ -5085,16 +5085,16 @@
     </row>
     <row r="162" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B162" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="B162" s="2" t="s">
-        <v>307</v>
-      </c>
       <c r="C162" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E162" s="1"/>
       <c r="F162" s="1"/>
@@ -5103,16 +5103,16 @@
     </row>
     <row r="163" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B163" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B163" s="2" t="s">
-        <v>309</v>
-      </c>
       <c r="C163" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E163" s="1"/>
       <c r="F163" s="1"/>
@@ -5121,16 +5121,16 @@
     </row>
     <row r="164" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B164" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B164" s="2" t="s">
-        <v>311</v>
-      </c>
       <c r="C164" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E164" s="1"/>
       <c r="F164" s="1"/>
@@ -5139,16 +5139,16 @@
     </row>
     <row r="165" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B165" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="B165" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="C165" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E165" s="1"/>
       <c r="F165" s="1"/>
@@ -5157,16 +5157,16 @@
     </row>
     <row r="166" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B166" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B166" s="2" t="s">
-        <v>315</v>
-      </c>
       <c r="C166" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E166" s="1"/>
       <c r="F166" s="1"/>
@@ -5175,16 +5175,16 @@
     </row>
     <row r="167" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B167" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="B167" s="2" t="s">
-        <v>317</v>
-      </c>
       <c r="C167" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E167" s="1"/>
       <c r="F167" s="1"/>
@@ -5193,10 +5193,10 @@
     </row>
     <row r="168" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B168" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>319</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>22</v>
@@ -5211,10 +5211,10 @@
     </row>
     <row r="169" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B169" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>22</v>
@@ -5229,16 +5229,16 @@
     </row>
     <row r="170" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B170" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B170" s="2" t="s">
-        <v>323</v>
-      </c>
       <c r="C170" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E170" s="1"/>
       <c r="F170" s="1"/>
@@ -5247,10 +5247,10 @@
     </row>
     <row r="171" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B171" s="2" t="s">
         <v>324</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>325</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>22</v>
@@ -5265,10 +5265,10 @@
     </row>
     <row r="172" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B172" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>327</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>22</v>
@@ -5283,16 +5283,16 @@
     </row>
     <row r="173" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B173" s="2" t="s">
-        <v>329</v>
-      </c>
       <c r="C173" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E173" s="1"/>
       <c r="F173" s="1"/>
@@ -5301,16 +5301,16 @@
     </row>
     <row r="174" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B174" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B174" s="2" t="s">
-        <v>331</v>
-      </c>
       <c r="C174" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E174" s="1"/>
       <c r="F174" s="1"/>
@@ -5319,10 +5319,10 @@
     </row>
     <row r="175" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>333</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>22</v>
@@ -5337,16 +5337,16 @@
     </row>
     <row r="176" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B176" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="B176" s="2" t="s">
-        <v>335</v>
-      </c>
       <c r="C176" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E176" s="1"/>
       <c r="F176" s="1"/>
@@ -5355,16 +5355,16 @@
     </row>
     <row r="177" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B177" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B177" s="2" t="s">
-        <v>337</v>
-      </c>
       <c r="C177" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E177" s="1"/>
       <c r="F177" s="1"/>
@@ -5373,7 +5373,7 @@
     </row>
     <row r="178" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>28</v>
@@ -5391,7 +5391,7 @@
     </row>
     <row r="179" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>28</v>
@@ -5409,16 +5409,16 @@
     </row>
     <row r="180" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B180" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B180" s="2" t="s">
-        <v>341</v>
-      </c>
       <c r="C180" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E180" s="1"/>
       <c r="F180" s="1"/>
@@ -5427,7 +5427,7 @@
     </row>
     <row r="181" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B181" s="2" t="s">
         <v>28</v>
@@ -5445,10 +5445,10 @@
     </row>
     <row r="182" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B182" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>344</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>22</v>
@@ -5463,7 +5463,7 @@
     </row>
     <row r="183" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B183" s="2" t="s">
         <v>28</v>
@@ -5481,10 +5481,10 @@
     </row>
     <row r="184" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B184" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>347</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>22</v>
@@ -5499,16 +5499,16 @@
     </row>
     <row r="185" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B185" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B185" s="2" t="s">
-        <v>349</v>
-      </c>
       <c r="C185" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E185" s="1"/>
       <c r="F185" s="1"/>
@@ -5517,10 +5517,10 @@
     </row>
     <row r="186" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B186" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>351</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>22</v>
@@ -5535,10 +5535,10 @@
     </row>
     <row r="187" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B187" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="B187" s="2" t="s">
-        <v>353</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>22</v>
@@ -5553,10 +5553,10 @@
     </row>
     <row r="188" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B188" s="2" t="s">
         <v>354</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>355</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>22</v>
@@ -5571,7 +5571,7 @@
     </row>
     <row r="189" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B189" s="2" t="s">
         <v>28</v>
@@ -5589,16 +5589,16 @@
     </row>
     <row r="190" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B190" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="B190" s="2" t="s">
-        <v>358</v>
-      </c>
       <c r="C190" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E190" s="1"/>
       <c r="F190" s="1"/>
@@ -5607,7 +5607,7 @@
     </row>
     <row r="191" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>28</v>
@@ -5625,16 +5625,16 @@
     </row>
     <row r="192" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B192" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="B192" s="2" t="s">
-        <v>361</v>
-      </c>
       <c r="C192" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E192" s="1"/>
       <c r="F192" s="1"/>
@@ -5643,16 +5643,16 @@
     </row>
     <row r="193" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B193" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B193" s="2" t="s">
-        <v>363</v>
-      </c>
       <c r="C193" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E193" s="1"/>
       <c r="F193" s="1"/>
@@ -5661,10 +5661,10 @@
     </row>
     <row r="194" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>365</v>
       </c>
       <c r="C194" s="2" t="s">
         <v>22</v>
@@ -5679,16 +5679,16 @@
     </row>
     <row r="195" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B195" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B195" s="2" t="s">
-        <v>367</v>
-      </c>
       <c r="C195" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E195" s="1"/>
       <c r="F195" s="1"/>
@@ -5697,16 +5697,16 @@
     </row>
     <row r="196" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B196" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="B196" s="2" t="s">
-        <v>369</v>
-      </c>
       <c r="C196" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E196" s="1"/>
       <c r="F196" s="1"/>
@@ -5715,36 +5715,36 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
+        <v>369</v>
+      </c>
+      <c r="B197" t="s">
         <v>370</v>
       </c>
-      <c r="B197" t="s">
+      <c r="C197" t="s">
         <v>371</v>
       </c>
-      <c r="C197" t="s">
-        <v>372</v>
-      </c>
       <c r="D197" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E197" t="s">
         <v>12</v>
       </c>
       <c r="G197" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="198" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B198" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B198" s="2" t="s">
-        <v>375</v>
-      </c>
       <c r="C198" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E198" s="1"/>
       <c r="F198" s="1"/>
@@ -5753,10 +5753,10 @@
     </row>
     <row r="199" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B199" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>377</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>22</v>
@@ -5771,7 +5771,7 @@
     </row>
     <row r="200" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>28</v>
@@ -5789,16 +5789,16 @@
     </row>
     <row r="201" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B201" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="B201" s="2" t="s">
-        <v>380</v>
-      </c>
       <c r="C201" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E201" s="1"/>
       <c r="F201" s="1"/>
@@ -5807,16 +5807,16 @@
     </row>
     <row r="202" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B202" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B202" s="2" t="s">
-        <v>382</v>
-      </c>
       <c r="C202" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E202" s="1"/>
       <c r="F202" s="1"/>
@@ -5825,7 +5825,7 @@
     </row>
     <row r="203" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>28</v>
@@ -5843,16 +5843,16 @@
     </row>
     <row r="204" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B204" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="B204" s="2" t="s">
-        <v>385</v>
-      </c>
       <c r="C204" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E204" s="1"/>
       <c r="F204" s="1"/>
@@ -5861,10 +5861,10 @@
     </row>
     <row r="205" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B205" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>22</v>
@@ -5879,10 +5879,10 @@
     </row>
     <row r="206" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B206" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="B206" s="2" t="s">
-        <v>389</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>22</v>
@@ -5897,7 +5897,7 @@
     </row>
     <row r="207" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>28</v>
@@ -5915,16 +5915,16 @@
     </row>
     <row r="208" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B208" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B208" s="2" t="s">
-        <v>392</v>
-      </c>
       <c r="C208" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E208" s="1"/>
       <c r="F208" s="1"/>
@@ -5933,16 +5933,16 @@
     </row>
     <row r="209" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B209" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B209" s="2" t="s">
-        <v>394</v>
-      </c>
       <c r="C209" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E209" s="1"/>
       <c r="F209" s="1"/>
@@ -5951,10 +5951,10 @@
     </row>
     <row r="210" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B210" s="2" t="s">
         <v>395</v>
-      </c>
-      <c r="B210" s="2" t="s">
-        <v>396</v>
       </c>
       <c r="C210" s="2" t="s">
         <v>22</v>
@@ -5969,16 +5969,16 @@
     </row>
     <row r="211" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B211" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B211" s="2" t="s">
-        <v>398</v>
-      </c>
       <c r="C211" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E211" s="1"/>
       <c r="F211" s="1"/>
@@ -5987,10 +5987,10 @@
     </row>
     <row r="212" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B212" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>400</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>22</v>
@@ -6005,16 +6005,16 @@
     </row>
     <row r="213" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B213" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="B213" s="2" t="s">
-        <v>402</v>
-      </c>
       <c r="C213" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E213" s="1"/>
       <c r="F213" s="1"/>
@@ -6023,7 +6023,7 @@
     </row>
     <row r="214" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B214" s="2" t="s">
         <v>28</v>
@@ -6041,10 +6041,10 @@
     </row>
     <row r="215" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B215" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="C215" s="2" t="s">
         <v>22</v>
@@ -6059,16 +6059,16 @@
     </row>
     <row r="216" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B216" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B216" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="C216" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E216" s="1"/>
       <c r="F216" s="1"/>
@@ -6077,16 +6077,16 @@
     </row>
     <row r="217" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B217" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B217" s="2" t="s">
-        <v>409</v>
-      </c>
       <c r="C217" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E217" s="1"/>
       <c r="F217" s="1"/>
@@ -6095,16 +6095,16 @@
     </row>
     <row r="218" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B218" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B218" s="2" t="s">
-        <v>411</v>
-      </c>
       <c r="C218" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E218" s="1"/>
       <c r="F218" s="1"/>
@@ -6113,16 +6113,16 @@
     </row>
     <row r="219" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E219" s="1"/>
       <c r="F219" s="1"/>
@@ -6131,10 +6131,10 @@
     </row>
     <row r="220" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B220" s="2" t="s">
         <v>413</v>
-      </c>
-      <c r="B220" s="2" t="s">
-        <v>414</v>
       </c>
       <c r="C220" s="2" t="s">
         <v>22</v>
@@ -6149,16 +6149,16 @@
     </row>
     <row r="221" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B221" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="B221" s="2" t="s">
-        <v>416</v>
-      </c>
       <c r="C221" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E221" s="1"/>
       <c r="F221" s="1"/>
@@ -6167,16 +6167,16 @@
     </row>
     <row r="222" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B222" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="B222" s="2" t="s">
-        <v>418</v>
-      </c>
       <c r="C222" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E222" s="1"/>
       <c r="F222" s="1"/>
@@ -6185,7 +6185,7 @@
     </row>
     <row r="223" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>28</v>
@@ -6203,7 +6203,7 @@
     </row>
     <row r="224" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>28</v>
@@ -6221,10 +6221,10 @@
     </row>
     <row r="225" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B225" s="2" t="s">
         <v>421</v>
-      </c>
-      <c r="B225" s="2" t="s">
-        <v>422</v>
       </c>
       <c r="C225" s="2" t="s">
         <v>22</v>
@@ -6239,16 +6239,16 @@
     </row>
     <row r="226" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B226" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="B226" s="2" t="s">
-        <v>424</v>
-      </c>
       <c r="C226" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E226" s="1"/>
       <c r="F226" s="1"/>
@@ -6257,7 +6257,7 @@
     </row>
     <row r="227" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B227" s="2" t="s">
         <v>28</v>

</xml_diff>